<commit_message>
#86 cardchange and buypiece now triggered by event
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/MainIcon.xlsx
+++ b/ConfigData/Xlsx/MainIcon.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17571"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\code\百度云同步盘\Trunk\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="36" windowWidth="18132" windowHeight="8388"/>
+    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
   </bookViews>
   <sheets>
     <sheet name="MainIcon" sheetId="1" r:id="rId1"/>
@@ -32,6 +32,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="宋体"/>
+            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t>real:</t>
@@ -41,6 +42,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="宋体"/>
+            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t xml:space="preserve">
@@ -56,6 +58,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="宋体"/>
+            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t>real:</t>
@@ -65,6 +68,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="宋体"/>
+            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t xml:space="preserve">
@@ -77,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="101">
   <si>
     <t>打开主菜单(ESC)</t>
   </si>
@@ -247,16 +251,10 @@
     <t>SideButton8</t>
   </si>
   <si>
-    <t>换卡</t>
-  </si>
-  <si>
     <t>[特有]随机交换卡片</t>
   </si>
   <si>
     <t>SideButton10</t>
-  </si>
-  <si>
-    <t>素材</t>
   </si>
   <si>
     <t>[特有]随机购买素材</t>
@@ -408,7 +406,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -592,6 +590,7 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
     </font>
     <font>
@@ -599,6 +598,7 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
     </font>
   </fonts>
@@ -1123,7 +1123,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1198,6 +1198,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1233,6 +1250,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1412,129 +1446,130 @@
   <dimension ref="A1:L30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="3" max="3" width="24.6640625" customWidth="1"/>
+    <col min="1" max="1" width="9" customWidth="1"/>
+    <col min="3" max="3" width="24.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C1" t="s">
         <v>88</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>89</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>90</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>91</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>92</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>93</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>94</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>95</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>96</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>97</v>
       </c>
-      <c r="K1" t="s">
-        <v>98</v>
-      </c>
-      <c r="L1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A3" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="J3" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="K3" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="L3" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="K3" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1569,7 +1604,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>2</v>
       </c>
@@ -1607,7 +1642,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>3</v>
       </c>
@@ -1645,7 +1680,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1683,7 +1718,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1721,7 +1756,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1759,7 +1794,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1797,7 +1832,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>11</v>
       </c>
@@ -1835,7 +1870,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>12</v>
       </c>
@@ -1873,7 +1908,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>32</v>
       </c>
@@ -1908,7 +1943,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>33</v>
       </c>
@@ -1943,7 +1978,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>34</v>
       </c>
@@ -1978,7 +2013,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>35</v>
       </c>
@@ -2016,7 +2051,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>36</v>
       </c>
@@ -2054,7 +2089,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>37</v>
       </c>
@@ -2092,7 +2127,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>38</v>
       </c>
@@ -2130,7 +2165,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A20">
         <v>39</v>
       </c>
@@ -2168,7 +2203,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A21">
         <v>40</v>
       </c>
@@ -2206,7 +2241,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A22">
         <v>41</v>
       </c>
@@ -2244,7 +2279,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A23">
         <v>42</v>
       </c>
@@ -2282,15 +2317,12 @@
         <v>55</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A24">
         <v>1000</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" t="s">
         <v>56</v>
-      </c>
-      <c r="C24" t="s">
-        <v>57</v>
       </c>
       <c r="D24">
         <v>0</v>
@@ -2317,18 +2349,15 @@
         <v>2</v>
       </c>
       <c r="L24" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A25">
         <v>1001</v>
       </c>
-      <c r="B25" t="s">
-        <v>59</v>
-      </c>
       <c r="C25" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D25">
         <v>0</v>
@@ -2355,18 +2384,18 @@
         <v>2</v>
       </c>
       <c r="L25" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A26">
         <v>1100</v>
       </c>
       <c r="B26" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C26" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D26">
         <v>0</v>
@@ -2393,18 +2422,18 @@
         <v>2</v>
       </c>
       <c r="L26" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A27">
         <v>1101</v>
       </c>
       <c r="B27" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C27" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D27">
         <v>0</v>
@@ -2431,18 +2460,18 @@
         <v>2</v>
       </c>
       <c r="L27" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A28">
         <v>1102</v>
       </c>
       <c r="B28" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C28" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D28">
         <v>0</v>
@@ -2469,18 +2498,18 @@
         <v>2</v>
       </c>
       <c r="L28" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A29">
         <v>1103</v>
       </c>
       <c r="B29" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C29" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D29">
         <v>0</v>
@@ -2507,18 +2536,18 @@
         <v>2</v>
       </c>
       <c r="L29" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A30">
         <v>1104</v>
       </c>
       <c r="B30" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C30" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D30">
         <v>0</v>
@@ -2545,7 +2574,7 @@
         <v>2</v>
       </c>
       <c r="L30" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
merge the mainicon and sceneconfig
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/MainIcon.xlsx
+++ b/ConfigData/Xlsx/MainIcon.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17571"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\code\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -81,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="98">
   <si>
     <t>打开主菜单(ESC)</t>
   </si>
@@ -204,15 +204,6 @@
   </si>
   <si>
     <t>SideButton5</t>
-  </si>
-  <si>
-    <t>休息</t>
-  </si>
-  <si>
-    <t>可以回复一定的体力值</t>
-  </si>
-  <si>
-    <t>SideButton4</t>
   </si>
   <si>
     <t>转盘</t>
@@ -406,7 +397,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1090,6 +1081,74 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1102,8 +1161,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:L30" totalsRowShown="0">
-  <autoFilter ref="A1:L30"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:L29" totalsRowShown="0">
+  <autoFilter ref="A1:L29"/>
   <tableColumns count="12">
     <tableColumn id="1" name="Id"/>
     <tableColumn id="2" name="Name"/>
@@ -1123,14 +1182,14 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="CAEACD"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -1198,23 +1257,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1250,23 +1292,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1443,10 +1468,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L30"/>
+  <dimension ref="A1:L29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1457,116 +1482,116 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1" t="s">
         <v>86</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" t="s">
         <v>87</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>88</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>89</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
         <v>90</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>91</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>92</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
         <v>93</v>
       </c>
-      <c r="I1" t="s">
+      <c r="L1" t="s">
         <v>94</v>
-      </c>
-      <c r="J1" t="s">
-        <v>95</v>
-      </c>
-      <c r="K1" t="s">
-        <v>96</v>
-      </c>
-      <c r="L1" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="J3" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="K3" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="L3" s="2" t="s">
         <v>82</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.15">
@@ -2129,7 +2154,7 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A19">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B19" t="s">
         <v>41</v>
@@ -2144,7 +2169,7 @@
         <v>0</v>
       </c>
       <c r="F19">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G19">
         <v>0</v>
@@ -2167,7 +2192,7 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A20">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B20" t="s">
         <v>44</v>
@@ -2176,13 +2201,13 @@
         <v>45</v>
       </c>
       <c r="D20">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E20">
-        <v>0</v>
+        <v>1100</v>
       </c>
       <c r="F20">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="G20">
         <v>0</v>
@@ -2205,7 +2230,7 @@
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A21">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B21" t="s">
         <v>47</v>
@@ -2214,13 +2239,13 @@
         <v>48</v>
       </c>
       <c r="D21">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E21">
-        <v>1100</v>
+        <v>1004</v>
       </c>
       <c r="F21">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="G21">
         <v>0</v>
@@ -2243,7 +2268,7 @@
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A22">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B22" t="s">
         <v>50</v>
@@ -2252,13 +2277,13 @@
         <v>51</v>
       </c>
       <c r="D22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E22">
-        <v>1004</v>
+        <v>0</v>
       </c>
       <c r="F22">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="G22">
         <v>0</v>
@@ -2273,7 +2298,7 @@
         <v>0</v>
       </c>
       <c r="K22">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L22" t="s">
         <v>52</v>
@@ -2281,48 +2306,45 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A23">
-        <v>42</v>
-      </c>
-      <c r="B23" t="s">
+        <v>1000</v>
+      </c>
+      <c r="C23" t="s">
         <v>53</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23">
+        <v>0</v>
+      </c>
+      <c r="J23">
+        <v>0</v>
+      </c>
+      <c r="K23">
+        <v>2</v>
+      </c>
+      <c r="L23" t="s">
         <v>54</v>
-      </c>
-      <c r="D23">
-        <v>0</v>
-      </c>
-      <c r="E23">
-        <v>0</v>
-      </c>
-      <c r="F23">
-        <v>50</v>
-      </c>
-      <c r="G23">
-        <v>0</v>
-      </c>
-      <c r="H23">
-        <v>0</v>
-      </c>
-      <c r="I23">
-        <v>0</v>
-      </c>
-      <c r="J23">
-        <v>0</v>
-      </c>
-      <c r="K23">
-        <v>3</v>
-      </c>
-      <c r="L23" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A24">
-        <v>1000</v>
+        <v>1001</v>
       </c>
       <c r="C24" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D24">
         <v>0</v>
@@ -2349,12 +2371,15 @@
         <v>2</v>
       </c>
       <c r="L24" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A25">
-        <v>1001</v>
+        <v>1100</v>
+      </c>
+      <c r="B25" t="s">
+        <v>57</v>
       </c>
       <c r="C25" t="s">
         <v>58</v>
@@ -2389,7 +2414,7 @@
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A26">
-        <v>1100</v>
+        <v>1101</v>
       </c>
       <c r="B26" t="s">
         <v>60</v>
@@ -2427,7 +2452,7 @@
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A27">
-        <v>1101</v>
+        <v>1102</v>
       </c>
       <c r="B27" t="s">
         <v>63</v>
@@ -2465,7 +2490,7 @@
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A28">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="B28" t="s">
         <v>66</v>
@@ -2503,13 +2528,13 @@
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A29">
-        <v>1103</v>
+        <v>1104</v>
       </c>
       <c r="B29" t="s">
-        <v>69</v>
+        <v>96</v>
       </c>
       <c r="C29" t="s">
-        <v>70</v>
+        <v>95</v>
       </c>
       <c r="D29">
         <v>0</v>
@@ -2536,45 +2561,7 @@
         <v>2</v>
       </c>
       <c r="L29" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A30">
-        <v>1104</v>
-      </c>
-      <c r="B30" t="s">
-        <v>99</v>
-      </c>
-      <c r="C30" t="s">
-        <v>98</v>
-      </c>
-      <c r="D30">
-        <v>0</v>
-      </c>
-      <c r="E30">
-        <v>0</v>
-      </c>
-      <c r="F30">
-        <v>0</v>
-      </c>
-      <c r="G30">
-        <v>0</v>
-      </c>
-      <c r="H30">
-        <v>0</v>
-      </c>
-      <c r="I30">
-        <v>0</v>
-      </c>
-      <c r="J30">
-        <v>0</v>
-      </c>
-      <c r="K30">
-        <v>2</v>
-      </c>
-      <c r="L30" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finish the equip compose function
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/MainIcon.xlsx
+++ b/ConfigData/Xlsx/MainIcon.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -81,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="101">
   <si>
     <t>打开主菜单(ESC)</t>
   </si>
@@ -391,6 +391,18 @@
   </si>
   <si>
     <t>SideButton18</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>合成</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>查看我的装备合成</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>MainIcon10</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1081,74 +1093,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1161,8 +1105,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:L29" totalsRowShown="0">
-  <autoFilter ref="A1:L29"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:L30" totalsRowShown="0">
+  <autoFilter ref="A1:L30"/>
   <tableColumns count="12">
     <tableColumn id="1" name="Id"/>
     <tableColumn id="2" name="Name"/>
@@ -1189,7 +1133,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="CAEACD"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -1468,10 +1412,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L29"/>
+  <dimension ref="A1:L30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1722,7 +1666,7 @@
         <v>0</v>
       </c>
       <c r="F7">
-        <v>0</v>
+        <v>99</v>
       </c>
       <c r="G7">
         <v>0</v>
@@ -1859,13 +1803,13 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A11">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>20</v>
+        <v>98</v>
       </c>
       <c r="C11" t="s">
-        <v>21</v>
+        <v>99</v>
       </c>
       <c r="D11">
         <v>0</v>
@@ -1874,7 +1818,7 @@
         <v>0</v>
       </c>
       <c r="F11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G11">
         <v>0</v>
@@ -1892,18 +1836,18 @@
         <v>1</v>
       </c>
       <c r="L11" t="s">
-        <v>22</v>
+        <v>100</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A12">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C12" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D12">
         <v>0</v>
@@ -1930,15 +1874,18 @@
         <v>1</v>
       </c>
       <c r="L12" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A13">
-        <v>32</v>
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>23</v>
       </c>
       <c r="C13" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D13">
         <v>0</v>
@@ -1950,30 +1897,30 @@
         <v>0</v>
       </c>
       <c r="G13">
-        <v>-184</v>
+        <v>0</v>
       </c>
       <c r="H13">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="I13">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="J13">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="K13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L13" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A14">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C14" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D14">
         <v>0</v>
@@ -1988,27 +1935,27 @@
         <v>-184</v>
       </c>
       <c r="H14">
-        <v>62</v>
+        <v>120</v>
       </c>
       <c r="I14">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="J14">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="K14">
         <v>0</v>
       </c>
       <c r="L14" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A15">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C15" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D15">
         <v>0</v>
@@ -2023,30 +1970,27 @@
         <v>-184</v>
       </c>
       <c r="H15">
-        <v>155</v>
+        <v>62</v>
       </c>
       <c r="I15">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="J15">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="K15">
         <v>0</v>
       </c>
       <c r="L15" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A16">
-        <v>35</v>
-      </c>
-      <c r="B16" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C16" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D16">
         <v>0</v>
@@ -2055,36 +1999,36 @@
         <v>0</v>
       </c>
       <c r="F16">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="G16">
-        <v>0</v>
+        <v>-184</v>
       </c>
       <c r="H16">
-        <v>0</v>
+        <v>155</v>
       </c>
       <c r="I16">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="J16">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="K16">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="L16" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A17">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B17" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C17" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D17">
         <v>0</v>
@@ -2093,7 +2037,7 @@
         <v>0</v>
       </c>
       <c r="F17">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="G17">
         <v>0</v>
@@ -2111,18 +2055,18 @@
         <v>3</v>
       </c>
       <c r="L17" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A18">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B18" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C18" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D18">
         <v>0</v>
@@ -2131,7 +2075,7 @@
         <v>0</v>
       </c>
       <c r="F18">
-        <v>99</v>
+        <v>20</v>
       </c>
       <c r="G18">
         <v>0</v>
@@ -2149,19 +2093,19 @@
         <v>3</v>
       </c>
       <c r="L18" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A19">
+        <v>37</v>
+      </c>
+      <c r="B19" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" t="s">
         <v>39</v>
       </c>
-      <c r="B19" t="s">
-        <v>41</v>
-      </c>
-      <c r="C19" t="s">
-        <v>42</v>
-      </c>
       <c r="D19">
         <v>0</v>
       </c>
@@ -2169,7 +2113,7 @@
         <v>0</v>
       </c>
       <c r="F19">
-        <v>5</v>
+        <v>99</v>
       </c>
       <c r="G19">
         <v>0</v>
@@ -2184,30 +2128,30 @@
         <v>0</v>
       </c>
       <c r="K19">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L19" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A20">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B20" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C20" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D20">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E20">
-        <v>1100</v>
+        <v>0</v>
       </c>
       <c r="F20">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G20">
         <v>0</v>
@@ -2225,27 +2169,27 @@
         <v>2</v>
       </c>
       <c r="L20" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A21">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B21" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C21" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D21">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E21">
-        <v>1004</v>
+        <v>1100</v>
       </c>
       <c r="F21">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="G21">
         <v>0</v>
@@ -2263,27 +2207,27 @@
         <v>2</v>
       </c>
       <c r="L21" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A22">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B22" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C22" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E22">
-        <v>0</v>
+        <v>1004</v>
       </c>
       <c r="F22">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="G22">
         <v>0</v>
@@ -2298,18 +2242,21 @@
         <v>0</v>
       </c>
       <c r="K22">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L22" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A23">
-        <v>1000</v>
+        <v>42</v>
+      </c>
+      <c r="B23" t="s">
+        <v>50</v>
       </c>
       <c r="C23" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D23">
         <v>0</v>
@@ -2318,7 +2265,7 @@
         <v>0</v>
       </c>
       <c r="F23">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="G23">
         <v>0</v>
@@ -2333,18 +2280,18 @@
         <v>0</v>
       </c>
       <c r="K23">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L23" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A24">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="C24" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D24">
         <v>0</v>
@@ -2371,18 +2318,15 @@
         <v>2</v>
       </c>
       <c r="L24" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A25">
-        <v>1100</v>
-      </c>
-      <c r="B25" t="s">
-        <v>57</v>
+        <v>1001</v>
       </c>
       <c r="C25" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D25">
         <v>0</v>
@@ -2409,18 +2353,18 @@
         <v>2</v>
       </c>
       <c r="L25" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A26">
-        <v>1101</v>
+        <v>1100</v>
       </c>
       <c r="B26" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C26" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D26">
         <v>0</v>
@@ -2447,18 +2391,18 @@
         <v>2</v>
       </c>
       <c r="L26" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A27">
-        <v>1102</v>
+        <v>1101</v>
       </c>
       <c r="B27" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C27" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D27">
         <v>0</v>
@@ -2485,18 +2429,18 @@
         <v>2</v>
       </c>
       <c r="L27" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A28">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="B28" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C28" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D28">
         <v>0</v>
@@ -2523,18 +2467,18 @@
         <v>2</v>
       </c>
       <c r="L28" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A29">
-        <v>1104</v>
+        <v>1103</v>
       </c>
       <c r="B29" t="s">
-        <v>96</v>
+        <v>66</v>
       </c>
       <c r="C29" t="s">
-        <v>95</v>
+        <v>67</v>
       </c>
       <c r="D29">
         <v>0</v>
@@ -2561,6 +2505,44 @@
         <v>2</v>
       </c>
       <c r="L29" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A30">
+        <v>1104</v>
+      </c>
+      <c r="B30" t="s">
+        <v>96</v>
+      </c>
+      <c r="C30" t="s">
+        <v>95</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30">
+        <v>0</v>
+      </c>
+      <c r="G30">
+        <v>0</v>
+      </c>
+      <c r="H30">
+        <v>0</v>
+      </c>
+      <c r="I30">
+        <v>0</v>
+      </c>
+      <c r="J30">
+        <v>0</v>
+      </c>
+      <c r="K30">
+        <v>2</v>
+      </c>
+      <c r="L30" t="s">
         <v>97</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add new structure farm
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/MainIcon.xlsx
+++ b/ConfigData/Xlsx/MainIcon.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -81,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="97">
   <si>
     <t>打开主菜单(ESC)</t>
   </si>
@@ -228,15 +228,6 @@
   </si>
   <si>
     <t>SideButton7</t>
-  </si>
-  <si>
-    <t>农场</t>
-  </si>
-  <si>
-    <t>打开农场面板</t>
-  </si>
-  <si>
-    <t>SideButton8</t>
   </si>
   <si>
     <t>[特有]随机交换卡片</t>
@@ -1090,74 +1081,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1170,8 +1093,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:L30" totalsRowShown="0">
-  <autoFilter ref="A1:L30"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:L29" totalsRowShown="0">
+  <autoFilter ref="A1:L29"/>
   <tableColumns count="12">
     <tableColumn id="1" name="Id"/>
     <tableColumn id="2" name="Name"/>
@@ -1198,7 +1121,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="CAEACD"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -1477,10 +1400,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L30"/>
+  <dimension ref="A1:L29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1494,116 +1417,116 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D1" t="s">
         <v>82</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" t="s">
         <v>83</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>84</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>85</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
         <v>86</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>87</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>88</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
         <v>89</v>
       </c>
-      <c r="I1" t="s">
+      <c r="L1" t="s">
         <v>90</v>
-      </c>
-      <c r="J1" t="s">
-        <v>91</v>
-      </c>
-      <c r="K1" t="s">
-        <v>92</v>
-      </c>
-      <c r="L1" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="J3" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="K3" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="L3" s="2" t="s">
         <v>78</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.15">
@@ -1874,10 +1797,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C11" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D11">
         <v>0</v>
@@ -1904,7 +1827,7 @@
         <v>1</v>
       </c>
       <c r="L11" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.15">
@@ -2315,48 +2238,45 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A23">
-        <v>42</v>
-      </c>
-      <c r="B23" t="s">
+        <v>1000</v>
+      </c>
+      <c r="C23" t="s">
         <v>49</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23">
+        <v>0</v>
+      </c>
+      <c r="J23">
+        <v>0</v>
+      </c>
+      <c r="K23">
+        <v>2</v>
+      </c>
+      <c r="L23" t="s">
         <v>50</v>
-      </c>
-      <c r="D23">
-        <v>0</v>
-      </c>
-      <c r="E23">
-        <v>0</v>
-      </c>
-      <c r="F23">
-        <v>50</v>
-      </c>
-      <c r="G23">
-        <v>0</v>
-      </c>
-      <c r="H23">
-        <v>0</v>
-      </c>
-      <c r="I23">
-        <v>0</v>
-      </c>
-      <c r="J23">
-        <v>0</v>
-      </c>
-      <c r="K23">
-        <v>3</v>
-      </c>
-      <c r="L23" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A24">
-        <v>1000</v>
+        <v>1001</v>
       </c>
       <c r="C24" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D24">
         <v>0</v>
@@ -2383,12 +2303,15 @@
         <v>2</v>
       </c>
       <c r="L24" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A25">
-        <v>1001</v>
+        <v>1100</v>
+      </c>
+      <c r="B25" t="s">
+        <v>53</v>
       </c>
       <c r="C25" t="s">
         <v>54</v>
@@ -2423,7 +2346,7 @@
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A26">
-        <v>1100</v>
+        <v>1101</v>
       </c>
       <c r="B26" t="s">
         <v>56</v>
@@ -2461,7 +2384,7 @@
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A27">
-        <v>1101</v>
+        <v>1102</v>
       </c>
       <c r="B27" t="s">
         <v>59</v>
@@ -2499,7 +2422,7 @@
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A28">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="B28" t="s">
         <v>62</v>
@@ -2537,13 +2460,13 @@
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A29">
-        <v>1103</v>
+        <v>1104</v>
       </c>
       <c r="B29" t="s">
-        <v>65</v>
+        <v>92</v>
       </c>
       <c r="C29" t="s">
-        <v>66</v>
+        <v>91</v>
       </c>
       <c r="D29">
         <v>0</v>
@@ -2570,45 +2493,7 @@
         <v>2</v>
       </c>
       <c r="L29" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A30">
-        <v>1104</v>
-      </c>
-      <c r="B30" t="s">
-        <v>95</v>
-      </c>
-      <c r="C30" t="s">
-        <v>94</v>
-      </c>
-      <c r="D30">
-        <v>0</v>
-      </c>
-      <c r="E30">
-        <v>0</v>
-      </c>
-      <c r="F30">
-        <v>0</v>
-      </c>
-      <c r="G30">
-        <v>0</v>
-      </c>
-      <c r="H30">
-        <v>0</v>
-      </c>
-      <c r="I30">
-        <v>0</v>
-      </c>
-      <c r="J30">
-        <v>0</v>
-      </c>
-      <c r="K30">
-        <v>2</v>
-      </c>
-      <c r="L30" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
remove the top icon flow
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/MainIcon.xlsx
+++ b/ConfigData/Xlsx/MainIcon.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="MainIcon" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -81,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="93">
   <si>
     <t>打开主菜单(ESC)</t>
   </si>
@@ -228,18 +228,6 @@
   </si>
   <si>
     <t>SideButton7</t>
-  </si>
-  <si>
-    <t>[特有]随机交换卡片</t>
-  </si>
-  <si>
-    <t>SideButton10</t>
-  </si>
-  <si>
-    <t>[特有]随机购买素材</t>
-  </si>
-  <si>
-    <t>SideButton11</t>
   </si>
   <si>
     <t>烹饪</t>
@@ -1093,8 +1081,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:L29" totalsRowShown="0">
-  <autoFilter ref="A1:L29"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:L27" totalsRowShown="0">
+  <autoFilter ref="A1:L27"/>
   <tableColumns count="12">
     <tableColumn id="1" name="Id"/>
     <tableColumn id="2" name="Name"/>
@@ -1400,10 +1388,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L29"/>
+  <dimension ref="A1:L27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="K17" sqref="K17:K27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1417,116 +1405,116 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E1" t="s">
         <v>79</v>
       </c>
-      <c r="B1" t="s">
+      <c r="F1" t="s">
         <v>80</v>
       </c>
-      <c r="C1" t="s">
+      <c r="G1" t="s">
         <v>81</v>
       </c>
-      <c r="D1" t="s">
+      <c r="H1" t="s">
         <v>82</v>
       </c>
-      <c r="E1" t="s">
+      <c r="I1" t="s">
         <v>83</v>
       </c>
-      <c r="F1" t="s">
+      <c r="J1" t="s">
         <v>84</v>
       </c>
-      <c r="G1" t="s">
+      <c r="K1" t="s">
         <v>85</v>
       </c>
-      <c r="H1" t="s">
+      <c r="L1" t="s">
         <v>86</v>
-      </c>
-      <c r="I1" t="s">
-        <v>87</v>
-      </c>
-      <c r="J1" t="s">
-        <v>88</v>
-      </c>
-      <c r="K1" t="s">
-        <v>89</v>
-      </c>
-      <c r="L1" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="J3" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="K3" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="L3" s="2" t="s">
         <v>74</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.15">
@@ -1797,10 +1785,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C11" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="D11">
         <v>0</v>
@@ -1827,7 +1815,7 @@
         <v>1</v>
       </c>
       <c r="L11" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.15">
@@ -2040,7 +2028,7 @@
         <v>0</v>
       </c>
       <c r="K17">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L17" t="s">
         <v>33</v>
@@ -2078,7 +2066,7 @@
         <v>0</v>
       </c>
       <c r="K18">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L18" t="s">
         <v>36</v>
@@ -2116,7 +2104,7 @@
         <v>0</v>
       </c>
       <c r="K19">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L19" t="s">
         <v>39</v>
@@ -2238,10 +2226,13 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A23">
-        <v>1000</v>
+        <v>1100</v>
+      </c>
+      <c r="B23" t="s">
+        <v>49</v>
       </c>
       <c r="C23" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D23">
         <v>0</v>
@@ -2268,15 +2259,18 @@
         <v>2</v>
       </c>
       <c r="L23" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A24">
-        <v>1001</v>
+        <v>1101</v>
+      </c>
+      <c r="B24" t="s">
+        <v>52</v>
       </c>
       <c r="C24" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D24">
         <v>0</v>
@@ -2303,18 +2297,18 @@
         <v>2</v>
       </c>
       <c r="L24" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A25">
-        <v>1100</v>
+        <v>1102</v>
       </c>
       <c r="B25" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C25" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D25">
         <v>0</v>
@@ -2341,18 +2335,18 @@
         <v>2</v>
       </c>
       <c r="L25" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A26">
-        <v>1101</v>
+        <v>1103</v>
       </c>
       <c r="B26" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C26" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D26">
         <v>0</v>
@@ -2379,18 +2373,18 @@
         <v>2</v>
       </c>
       <c r="L26" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A27">
-        <v>1102</v>
+        <v>1104</v>
       </c>
       <c r="B27" t="s">
-        <v>59</v>
+        <v>88</v>
       </c>
       <c r="C27" t="s">
-        <v>60</v>
+        <v>87</v>
       </c>
       <c r="D27">
         <v>0</v>
@@ -2417,83 +2411,7 @@
         <v>2</v>
       </c>
       <c r="L27" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A28">
-        <v>1103</v>
-      </c>
-      <c r="B28" t="s">
-        <v>62</v>
-      </c>
-      <c r="C28" t="s">
-        <v>63</v>
-      </c>
-      <c r="D28">
-        <v>0</v>
-      </c>
-      <c r="E28">
-        <v>0</v>
-      </c>
-      <c r="F28">
-        <v>0</v>
-      </c>
-      <c r="G28">
-        <v>0</v>
-      </c>
-      <c r="H28">
-        <v>0</v>
-      </c>
-      <c r="I28">
-        <v>0</v>
-      </c>
-      <c r="J28">
-        <v>0</v>
-      </c>
-      <c r="K28">
-        <v>2</v>
-      </c>
-      <c r="L28" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A29">
-        <v>1104</v>
-      </c>
-      <c r="B29" t="s">
-        <v>92</v>
-      </c>
-      <c r="C29" t="s">
-        <v>91</v>
-      </c>
-      <c r="D29">
-        <v>0</v>
-      </c>
-      <c r="E29">
-        <v>0</v>
-      </c>
-      <c r="F29">
-        <v>0</v>
-      </c>
-      <c r="G29">
-        <v>0</v>
-      </c>
-      <c r="H29">
-        <v>0</v>
-      </c>
-      <c r="I29">
-        <v>0</v>
-      </c>
-      <c r="J29">
-        <v>0</v>
-      </c>
-      <c r="K29">
-        <v>2</v>
-      </c>
-      <c r="L29" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#100 a basicly quest form
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/MainIcon.xlsx
+++ b/ConfigData/Xlsx/MainIcon.xlsx
@@ -107,12 +107,6 @@
     <t>MainIcon9</t>
   </si>
   <si>
-    <t>任务</t>
-  </si>
-  <si>
-    <t>打开任务日志(T)</t>
-  </si>
-  <si>
     <t>MainIcon3</t>
   </si>
   <si>
@@ -379,6 +373,14 @@
   </si>
   <si>
     <t>MainIcon10</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>传记</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>查看自己的传记(T)</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1391,7 +1393,7 @@
   <dimension ref="A1:L27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17:K27"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1405,116 +1407,116 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1" t="s">
         <v>75</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>76</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>77</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>78</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>79</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>80</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>81</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>82</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>83</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>84</v>
-      </c>
-      <c r="K1" t="s">
-        <v>85</v>
-      </c>
-      <c r="L1" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="J3" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="K3" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="L3" s="2" t="s">
         <v>72</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.15">
@@ -1633,10 +1635,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>91</v>
       </c>
       <c r="C7" t="s">
-        <v>9</v>
+        <v>92</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -1645,7 +1647,7 @@
         <v>0</v>
       </c>
       <c r="F7">
-        <v>99</v>
+        <v>0</v>
       </c>
       <c r="G7">
         <v>0</v>
@@ -1663,7 +1665,7 @@
         <v>1</v>
       </c>
       <c r="L7" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.15">
@@ -1671,10 +1673,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -1701,7 +1703,7 @@
         <v>1</v>
       </c>
       <c r="L8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.15">
@@ -1709,10 +1711,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C9" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -1739,7 +1741,7 @@
         <v>1</v>
       </c>
       <c r="L9" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.15">
@@ -1747,10 +1749,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -1777,7 +1779,7 @@
         <v>1</v>
       </c>
       <c r="L10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.15">
@@ -1785,10 +1787,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C11" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D11">
         <v>0</v>
@@ -1815,7 +1817,7 @@
         <v>1</v>
       </c>
       <c r="L11" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.15">
@@ -1823,10 +1825,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C12" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D12">
         <v>0</v>
@@ -1853,7 +1855,7 @@
         <v>1</v>
       </c>
       <c r="L12" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.15">
@@ -1861,10 +1863,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C13" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D13">
         <v>0</v>
@@ -1891,7 +1893,7 @@
         <v>1</v>
       </c>
       <c r="L13" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.15">
@@ -1899,7 +1901,7 @@
         <v>32</v>
       </c>
       <c r="C14" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D14">
         <v>0</v>
@@ -1926,7 +1928,7 @@
         <v>0</v>
       </c>
       <c r="L14" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.15">
@@ -1934,7 +1936,7 @@
         <v>33</v>
       </c>
       <c r="C15" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D15">
         <v>0</v>
@@ -1961,7 +1963,7 @@
         <v>0</v>
       </c>
       <c r="L15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.15">
@@ -1969,7 +1971,7 @@
         <v>34</v>
       </c>
       <c r="C16" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D16">
         <v>0</v>
@@ -1996,7 +1998,7 @@
         <v>0</v>
       </c>
       <c r="L16" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.15">
@@ -2004,7 +2006,7 @@
         <v>35</v>
       </c>
       <c r="C17" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D17">
         <v>0</v>
@@ -2031,7 +2033,7 @@
         <v>2</v>
       </c>
       <c r="L17" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.15">
@@ -2039,10 +2041,10 @@
         <v>36</v>
       </c>
       <c r="B18" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C18" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D18">
         <v>0</v>
@@ -2069,7 +2071,7 @@
         <v>2</v>
       </c>
       <c r="L18" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.15">
@@ -2077,10 +2079,10 @@
         <v>37</v>
       </c>
       <c r="B19" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C19" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D19">
         <v>0</v>
@@ -2107,7 +2109,7 @@
         <v>2</v>
       </c>
       <c r="L19" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.15">
@@ -2115,10 +2117,10 @@
         <v>39</v>
       </c>
       <c r="B20" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C20" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D20">
         <v>0</v>
@@ -2145,7 +2147,7 @@
         <v>2</v>
       </c>
       <c r="L20" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.15">
@@ -2153,10 +2155,10 @@
         <v>40</v>
       </c>
       <c r="B21" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C21" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D21">
         <v>2</v>
@@ -2183,7 +2185,7 @@
         <v>2</v>
       </c>
       <c r="L21" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.15">
@@ -2191,10 +2193,10 @@
         <v>41</v>
       </c>
       <c r="B22" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C22" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D22">
         <v>1</v>
@@ -2221,7 +2223,7 @@
         <v>2</v>
       </c>
       <c r="L22" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.15">
@@ -2229,10 +2231,10 @@
         <v>1100</v>
       </c>
       <c r="B23" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C23" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D23">
         <v>0</v>
@@ -2259,7 +2261,7 @@
         <v>2</v>
       </c>
       <c r="L23" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.15">
@@ -2267,10 +2269,10 @@
         <v>1101</v>
       </c>
       <c r="B24" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C24" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D24">
         <v>0</v>
@@ -2297,7 +2299,7 @@
         <v>2</v>
       </c>
       <c r="L24" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.15">
@@ -2305,10 +2307,10 @@
         <v>1102</v>
       </c>
       <c r="B25" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C25" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D25">
         <v>0</v>
@@ -2335,7 +2337,7 @@
         <v>2</v>
       </c>
       <c r="L25" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.15">
@@ -2343,10 +2345,10 @@
         <v>1103</v>
       </c>
       <c r="B26" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C26" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D26">
         <v>0</v>
@@ -2373,7 +2375,7 @@
         <v>2</v>
       </c>
       <c r="L26" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.15">
@@ -2381,10 +2383,10 @@
         <v>1104</v>
       </c>
       <c r="B27" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C27" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D27">
         <v>0</v>
@@ -2411,7 +2413,7 @@
         <v>2</v>
       </c>
       <c r="L27" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add a minigame form
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/MainIcon.xlsx
+++ b/ConfigData/Xlsx/MainIcon.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\Code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -81,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="95">
   <si>
     <t>打开主菜单(ESC)</t>
   </si>
@@ -381,6 +381,14 @@
   </si>
   <si>
     <t>查看自己的传记(T)</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>游戏</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>打开迷你游戏面板</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1071,6 +1079,74 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1083,8 +1159,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:L27" totalsRowShown="0">
-  <autoFilter ref="A1:L27"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:L28" totalsRowShown="0">
+  <autoFilter ref="A1:L28"/>
   <tableColumns count="12">
     <tableColumn id="1" name="Id"/>
     <tableColumn id="2" name="Name"/>
@@ -1111,7 +1187,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="CAEACD"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -1390,10 +1466,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L27"/>
+  <dimension ref="A1:L28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2228,13 +2304,13 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A23">
-        <v>1100</v>
+        <v>42</v>
       </c>
       <c r="B23" t="s">
-        <v>47</v>
+        <v>93</v>
       </c>
       <c r="C23" t="s">
-        <v>48</v>
+        <v>94</v>
       </c>
       <c r="D23">
         <v>0</v>
@@ -2261,18 +2337,18 @@
         <v>2</v>
       </c>
       <c r="L23" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A24">
-        <v>1101</v>
+        <v>1100</v>
       </c>
       <c r="B24" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C24" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D24">
         <v>0</v>
@@ -2299,18 +2375,18 @@
         <v>2</v>
       </c>
       <c r="L24" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A25">
-        <v>1102</v>
+        <v>1101</v>
       </c>
       <c r="B25" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C25" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D25">
         <v>0</v>
@@ -2337,18 +2413,18 @@
         <v>2</v>
       </c>
       <c r="L25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A26">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="B26" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C26" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D26">
         <v>0</v>
@@ -2375,18 +2451,18 @@
         <v>2</v>
       </c>
       <c r="L26" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A27">
-        <v>1104</v>
+        <v>1103</v>
       </c>
       <c r="B27" t="s">
-        <v>86</v>
+        <v>56</v>
       </c>
       <c r="C27" t="s">
-        <v>85</v>
+        <v>57</v>
       </c>
       <c r="D27">
         <v>0</v>
@@ -2413,6 +2489,44 @@
         <v>2</v>
       </c>
       <c r="L27" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A28">
+        <v>1104</v>
+      </c>
+      <c r="B28" t="s">
+        <v>86</v>
+      </c>
+      <c r="C28" t="s">
+        <v>85</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28">
+        <v>0</v>
+      </c>
+      <c r="G28">
+        <v>0</v>
+      </c>
+      <c r="H28">
+        <v>0</v>
+      </c>
+      <c r="I28">
+        <v>0</v>
+      </c>
+      <c r="J28">
+        <v>0</v>
+      </c>
+      <c r="K28">
+        <v>2</v>
+      </c>
+      <c r="L28" t="s">
         <v>87</v>
       </c>
     </row>

</xml_diff>

<commit_message>
basically integrade the linegame
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/MainIcon.xlsx
+++ b/ConfigData/Xlsx/MainIcon.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\Code\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -81,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="96">
   <si>
     <t>打开主菜单(ESC)</t>
   </si>
@@ -389,6 +389,10 @@
   </si>
   <si>
     <t>打开迷你游戏面板</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>SideButton4</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1079,74 +1083,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1187,7 +1123,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="CAEACD"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -1469,7 +1405,7 @@
   <dimension ref="A1:L28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2337,7 +2273,7 @@
         <v>2</v>
       </c>
       <c r="L23" t="s">
-        <v>46</v>
+        <v>95</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
remake the equip wear logic
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/MainIcon.xlsx
+++ b/ConfigData/Xlsx/MainIcon.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18067"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TOMClassic\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -146,12 +146,6 @@
     <t>MainIcon2</t>
   </si>
   <si>
-    <t>角色</t>
-  </si>
-  <si>
-    <t>查看玩家的状态(C)</t>
-  </si>
-  <si>
     <t>MainIcon4</t>
   </si>
   <si>
@@ -345,6 +339,14 @@
   </si>
   <si>
     <t>SideButton4</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>城堡</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>查看城堡的状态(C)</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1391,7 +1393,7 @@
   <dimension ref="A1:L23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24:XFD28"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1405,116 +1407,116 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1" t="s">
         <v>61</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>62</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>63</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>64</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>65</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>66</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>67</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>68</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>69</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>70</v>
-      </c>
-      <c r="K1" t="s">
-        <v>71</v>
-      </c>
-      <c r="L1" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="J3" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="K3" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="L3" s="2" t="s">
         <v>58</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.15">
@@ -1633,10 +1635,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -1785,10 +1787,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C11" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D11">
         <v>0</v>
@@ -1815,7 +1817,7 @@
         <v>1</v>
       </c>
       <c r="L11" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.15">
@@ -1861,10 +1863,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>21</v>
+        <v>79</v>
       </c>
       <c r="C13" t="s">
-        <v>22</v>
+        <v>80</v>
       </c>
       <c r="D13">
         <v>0</v>
@@ -1891,7 +1893,7 @@
         <v>1</v>
       </c>
       <c r="L13" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.15">
@@ -1899,7 +1901,7 @@
         <v>32</v>
       </c>
       <c r="C14" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D14">
         <v>0</v>
@@ -1926,7 +1928,7 @@
         <v>0</v>
       </c>
       <c r="L14" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.15">
@@ -1934,7 +1936,7 @@
         <v>33</v>
       </c>
       <c r="C15" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D15">
         <v>0</v>
@@ -1961,7 +1963,7 @@
         <v>0</v>
       </c>
       <c r="L15" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.15">
@@ -1969,7 +1971,7 @@
         <v>34</v>
       </c>
       <c r="C16" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D16">
         <v>0</v>
@@ -1996,7 +1998,7 @@
         <v>0</v>
       </c>
       <c r="L16" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.15">
@@ -2004,7 +2006,7 @@
         <v>35</v>
       </c>
       <c r="C17" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D17">
         <v>0</v>
@@ -2031,7 +2033,7 @@
         <v>2</v>
       </c>
       <c r="L17" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.15">
@@ -2039,10 +2041,10 @@
         <v>36</v>
       </c>
       <c r="B18" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C18" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D18">
         <v>0</v>
@@ -2069,7 +2071,7 @@
         <v>2</v>
       </c>
       <c r="L18" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.15">
@@ -2077,10 +2079,10 @@
         <v>37</v>
       </c>
       <c r="B19" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C19" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D19">
         <v>0</v>
@@ -2107,7 +2109,7 @@
         <v>2</v>
       </c>
       <c r="L19" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.15">
@@ -2115,10 +2117,10 @@
         <v>39</v>
       </c>
       <c r="B20" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C20" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D20">
         <v>0</v>
@@ -2145,7 +2147,7 @@
         <v>2</v>
       </c>
       <c r="L20" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.15">
@@ -2153,10 +2155,10 @@
         <v>40</v>
       </c>
       <c r="B21" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C21" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D21">
         <v>2</v>
@@ -2183,7 +2185,7 @@
         <v>2</v>
       </c>
       <c r="L21" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.15">
@@ -2191,10 +2193,10 @@
         <v>41</v>
       </c>
       <c r="B22" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C22" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D22">
         <v>1</v>
@@ -2221,7 +2223,7 @@
         <v>2</v>
       </c>
       <c r="L22" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.15">
@@ -2229,10 +2231,10 @@
         <v>42</v>
       </c>
       <c r="B23" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C23" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D23">
         <v>0</v>
@@ -2259,7 +2261,7 @@
         <v>2</v>
       </c>
       <c r="L23" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fill the equip data
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/MainIcon.xlsx
+++ b/ConfigData/Xlsx/MainIcon.xlsx
@@ -310,14 +310,6 @@
     <t>Icon</t>
   </si>
   <si>
-    <t>合成</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>查看我的装备合成</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>MainIcon10</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -347,6 +339,14 @@
   </si>
   <si>
     <t>查看城堡的状态(C)</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>建造</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>查看我的建造目录</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1393,7 +1393,7 @@
   <dimension ref="A1:L23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1635,10 +1635,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C7" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -1787,10 +1787,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="C11" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="D11">
         <v>0</v>
@@ -1817,7 +1817,7 @@
         <v>1</v>
       </c>
       <c r="L11" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.15">
@@ -1863,10 +1863,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C13" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D13">
         <v>0</v>
@@ -2231,10 +2231,10 @@
         <v>42</v>
       </c>
       <c r="B23" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C23" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D23">
         <v>0</v>
@@ -2261,7 +2261,7 @@
         <v>2</v>
       </c>
       <c r="L23" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
remove the quest system, to make a sandbox task system
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/MainIcon.xlsx
+++ b/ConfigData/Xlsx/MainIcon.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18067"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18229"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Code\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TOMClassic\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -81,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="72">
   <si>
     <t>打开主菜单(ESC)</t>
   </si>
@@ -105,9 +105,6 @@
   </si>
   <si>
     <t>MainIcon9</t>
-  </si>
-  <si>
-    <t>MainIcon3</t>
   </si>
   <si>
     <t>挑战</t>
@@ -293,14 +290,6 @@
   </si>
   <si>
     <t>MainIcon10</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>传记</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>查看自己的传记(T)</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
@@ -1031,8 +1020,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:L21" totalsRowShown="0">
-  <autoFilter ref="A1:L21"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:L20" totalsRowShown="0">
+  <autoFilter ref="A1:L20"/>
   <tableColumns count="12">
     <tableColumn id="1" name="Id"/>
     <tableColumn id="2" name="Name"/>
@@ -1372,10 +1361,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L21"/>
+  <dimension ref="A1:L20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1389,116 +1378,116 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" t="s">
         <v>53</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>54</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>55</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>56</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>57</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>58</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>59</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>60</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>61</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>62</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>63</v>
-      </c>
-      <c r="L1" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>40</v>
-      </c>
       <c r="C2" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="L2" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="J3" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="K3" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="L3" s="2" t="s">
         <v>51</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.15">
@@ -1614,13 +1603,13 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A7">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>66</v>
+        <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>67</v>
+        <v>9</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -1629,7 +1618,7 @@
         <v>0</v>
       </c>
       <c r="F7">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G7">
         <v>0</v>
@@ -1647,18 +1636,18 @@
         <v>1</v>
       </c>
       <c r="L7" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A8">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -1667,7 +1656,7 @@
         <v>0</v>
       </c>
       <c r="F8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G8">
         <v>0</v>
@@ -1685,18 +1674,18 @@
         <v>1</v>
       </c>
       <c r="L8" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A9">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>70</v>
       </c>
       <c r="C9" t="s">
-        <v>13</v>
+        <v>71</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -1705,7 +1694,7 @@
         <v>0</v>
       </c>
       <c r="F9">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="G9">
         <v>0</v>
@@ -1723,18 +1712,18 @@
         <v>1</v>
       </c>
       <c r="L9" t="s">
-        <v>14</v>
+        <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A10">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>73</v>
+        <v>14</v>
       </c>
       <c r="C10" t="s">
-        <v>74</v>
+        <v>15</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -1743,7 +1732,7 @@
         <v>0</v>
       </c>
       <c r="F10">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="G10">
         <v>0</v>
@@ -1761,18 +1750,18 @@
         <v>1</v>
       </c>
       <c r="L10" t="s">
-        <v>65</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A11">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>15</v>
+        <v>68</v>
       </c>
       <c r="C11" t="s">
-        <v>16</v>
+        <v>69</v>
       </c>
       <c r="D11">
         <v>0</v>
@@ -1804,13 +1793,10 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A12">
-        <v>12</v>
-      </c>
-      <c r="B12" t="s">
-        <v>71</v>
+        <v>32</v>
       </c>
       <c r="C12" t="s">
-        <v>72</v>
+        <v>18</v>
       </c>
       <c r="D12">
         <v>0</v>
@@ -1822,30 +1808,30 @@
         <v>0</v>
       </c>
       <c r="G12">
-        <v>0</v>
+        <v>-184</v>
       </c>
       <c r="H12">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="I12">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="J12">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="K12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L12" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A13">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C13" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D13">
         <v>0</v>
@@ -1860,27 +1846,27 @@
         <v>-184</v>
       </c>
       <c r="H13">
-        <v>120</v>
+        <v>62</v>
       </c>
       <c r="I13">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="J13">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="K13">
         <v>0</v>
       </c>
       <c r="L13" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A14">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C14" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D14">
         <v>0</v>
@@ -1895,27 +1881,27 @@
         <v>-184</v>
       </c>
       <c r="H14">
-        <v>62</v>
+        <v>155</v>
       </c>
       <c r="I14">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="J14">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="K14">
         <v>0</v>
       </c>
       <c r="L14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A15">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C15" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D15">
         <v>0</v>
@@ -1924,33 +1910,36 @@
         <v>0</v>
       </c>
       <c r="F15">
-        <v>0</v>
+        <v>99</v>
       </c>
       <c r="G15">
-        <v>-184</v>
+        <v>0</v>
       </c>
       <c r="H15">
-        <v>155</v>
+        <v>0</v>
       </c>
       <c r="I15">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="J15">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="K15">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L15" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A16">
-        <v>35</v>
+        <v>36</v>
+      </c>
+      <c r="B16" t="s">
+        <v>26</v>
       </c>
       <c r="C16" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D16">
         <v>0</v>
@@ -1959,7 +1948,7 @@
         <v>0</v>
       </c>
       <c r="F16">
-        <v>99</v>
+        <v>20</v>
       </c>
       <c r="G16">
         <v>0</v>
@@ -1977,18 +1966,18 @@
         <v>2</v>
       </c>
       <c r="L16" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A17">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B17" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C17" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D17">
         <v>0</v>
@@ -1997,7 +1986,7 @@
         <v>0</v>
       </c>
       <c r="F17">
-        <v>20</v>
+        <v>99</v>
       </c>
       <c r="G17">
         <v>0</v>
@@ -2015,18 +2004,18 @@
         <v>2</v>
       </c>
       <c r="L17" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A18">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B18" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C18" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D18">
         <v>0</v>
@@ -2035,7 +2024,7 @@
         <v>0</v>
       </c>
       <c r="F18">
-        <v>99</v>
+        <v>12</v>
       </c>
       <c r="G18">
         <v>0</v>
@@ -2053,27 +2042,27 @@
         <v>2</v>
       </c>
       <c r="L18" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A19">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B19" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C19" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E19">
-        <v>0</v>
+        <v>1004</v>
       </c>
       <c r="F19">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="G19">
         <v>0</v>
@@ -2091,27 +2080,27 @@
         <v>2</v>
       </c>
       <c r="L19" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A20">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B20" t="s">
-        <v>36</v>
+        <v>65</v>
       </c>
       <c r="C20" t="s">
-        <v>37</v>
+        <v>66</v>
       </c>
       <c r="D20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E20">
-        <v>1004</v>
+        <v>0</v>
       </c>
       <c r="F20">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="G20">
         <v>0</v>
@@ -2129,45 +2118,7 @@
         <v>2</v>
       </c>
       <c r="L20" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A21">
-        <v>42</v>
-      </c>
-      <c r="B21" t="s">
-        <v>68</v>
-      </c>
-      <c r="C21" t="s">
-        <v>69</v>
-      </c>
-      <c r="D21">
-        <v>0</v>
-      </c>
-      <c r="E21">
-        <v>0</v>
-      </c>
-      <c r="F21">
-        <v>0</v>
-      </c>
-      <c r="G21">
-        <v>0</v>
-      </c>
-      <c r="H21">
-        <v>0</v>
-      </c>
-      <c r="I21">
-        <v>0</v>
-      </c>
-      <c r="J21">
-        <v>0</v>
-      </c>
-      <c r="K21">
-        <v>2</v>
-      </c>
-      <c r="L21" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add back the quest config
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/MainIcon.xlsx
+++ b/ConfigData/Xlsx/MainIcon.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18229"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18067"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TOMClassic\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -81,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="75">
   <si>
     <t>打开主菜单(ESC)</t>
   </si>
@@ -107,6 +107,9 @@
     <t>MainIcon9</t>
   </si>
   <si>
+    <t>MainIcon3</t>
+  </si>
+  <si>
     <t>挑战</t>
   </si>
   <si>
@@ -290,6 +293,14 @@
   </si>
   <si>
     <t>MainIcon10</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>传记</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>查看自己的传记(T)</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
@@ -1020,8 +1031,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:L20" totalsRowShown="0">
-  <autoFilter ref="A1:L20"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:L21" totalsRowShown="0">
+  <autoFilter ref="A1:L21"/>
   <tableColumns count="12">
     <tableColumn id="1" name="Id"/>
     <tableColumn id="2" name="Name"/>
@@ -1361,10 +1372,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L20"/>
+  <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1378,116 +1389,116 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="I1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="J1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="K1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="L1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>38</v>
-      </c>
       <c r="F2" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.15">
@@ -1603,13 +1614,13 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A7">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>66</v>
       </c>
       <c r="C7" t="s">
-        <v>9</v>
+        <v>67</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -1618,7 +1629,7 @@
         <v>0</v>
       </c>
       <c r="F7">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G7">
         <v>0</v>
@@ -1636,18 +1647,18 @@
         <v>1</v>
       </c>
       <c r="L7" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A8">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -1656,7 +1667,7 @@
         <v>0</v>
       </c>
       <c r="F8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G8">
         <v>0</v>
@@ -1674,18 +1685,18 @@
         <v>1</v>
       </c>
       <c r="L8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A9">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>70</v>
+        <v>12</v>
       </c>
       <c r="C9" t="s">
-        <v>71</v>
+        <v>13</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -1694,7 +1705,7 @@
         <v>0</v>
       </c>
       <c r="F9">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="G9">
         <v>0</v>
@@ -1712,18 +1723,18 @@
         <v>1</v>
       </c>
       <c r="L9" t="s">
-        <v>64</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A10">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>14</v>
+        <v>73</v>
       </c>
       <c r="C10" t="s">
-        <v>15</v>
+        <v>74</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -1732,7 +1743,7 @@
         <v>0</v>
       </c>
       <c r="F10">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G10">
         <v>0</v>
@@ -1750,18 +1761,18 @@
         <v>1</v>
       </c>
       <c r="L10" t="s">
-        <v>16</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A11">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>68</v>
+        <v>15</v>
       </c>
       <c r="C11" t="s">
-        <v>69</v>
+        <v>16</v>
       </c>
       <c r="D11">
         <v>0</v>
@@ -1793,45 +1804,48 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A12">
-        <v>32</v>
+        <v>12</v>
+      </c>
+      <c r="B12" t="s">
+        <v>71</v>
       </c>
       <c r="C12" t="s">
+        <v>72</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>1</v>
+      </c>
+      <c r="L12" t="s">
         <v>18</v>
-      </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-      <c r="E12">
-        <v>0</v>
-      </c>
-      <c r="F12">
-        <v>0</v>
-      </c>
-      <c r="G12">
-        <v>-184</v>
-      </c>
-      <c r="H12">
-        <v>120</v>
-      </c>
-      <c r="I12">
-        <v>28</v>
-      </c>
-      <c r="J12">
-        <v>28</v>
-      </c>
-      <c r="K12">
-        <v>0</v>
-      </c>
-      <c r="L12" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A13">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D13">
         <v>0</v>
@@ -1846,27 +1860,27 @@
         <v>-184</v>
       </c>
       <c r="H13">
-        <v>62</v>
+        <v>120</v>
       </c>
       <c r="I13">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="J13">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="K13">
         <v>0</v>
       </c>
       <c r="L13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A14">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D14">
         <v>0</v>
@@ -1881,65 +1895,62 @@
         <v>-184</v>
       </c>
       <c r="H14">
-        <v>155</v>
+        <v>62</v>
       </c>
       <c r="I14">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="J14">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="K14">
         <v>0</v>
       </c>
       <c r="L14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A15">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C15" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>-184</v>
+      </c>
+      <c r="H15">
+        <v>155</v>
+      </c>
+      <c r="I15">
+        <v>28</v>
+      </c>
+      <c r="J15">
+        <v>28</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="L15" t="s">
         <v>24</v>
-      </c>
-      <c r="D15">
-        <v>0</v>
-      </c>
-      <c r="E15">
-        <v>0</v>
-      </c>
-      <c r="F15">
-        <v>99</v>
-      </c>
-      <c r="G15">
-        <v>0</v>
-      </c>
-      <c r="H15">
-        <v>0</v>
-      </c>
-      <c r="I15">
-        <v>0</v>
-      </c>
-      <c r="J15">
-        <v>0</v>
-      </c>
-      <c r="K15">
-        <v>2</v>
-      </c>
-      <c r="L15" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A16">
-        <v>36</v>
-      </c>
-      <c r="B16" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="C16" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D16">
         <v>0</v>
@@ -1948,7 +1959,7 @@
         <v>0</v>
       </c>
       <c r="F16">
-        <v>20</v>
+        <v>99</v>
       </c>
       <c r="G16">
         <v>0</v>
@@ -1966,18 +1977,18 @@
         <v>2</v>
       </c>
       <c r="L16" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A17">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B17" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C17" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D17">
         <v>0</v>
@@ -1986,7 +1997,7 @@
         <v>0</v>
       </c>
       <c r="F17">
-        <v>99</v>
+        <v>20</v>
       </c>
       <c r="G17">
         <v>0</v>
@@ -2004,18 +2015,18 @@
         <v>2</v>
       </c>
       <c r="L17" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A18">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B18" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C18" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D18">
         <v>0</v>
@@ -2024,7 +2035,7 @@
         <v>0</v>
       </c>
       <c r="F18">
-        <v>12</v>
+        <v>99</v>
       </c>
       <c r="G18">
         <v>0</v>
@@ -2042,27 +2053,27 @@
         <v>2</v>
       </c>
       <c r="L18" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A19">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B19" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C19" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E19">
-        <v>1004</v>
+        <v>0</v>
       </c>
       <c r="F19">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="G19">
         <v>0</v>
@@ -2080,27 +2091,27 @@
         <v>2</v>
       </c>
       <c r="L19" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A20">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B20" t="s">
-        <v>65</v>
+        <v>36</v>
       </c>
       <c r="C20" t="s">
-        <v>66</v>
+        <v>37</v>
       </c>
       <c r="D20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E20">
-        <v>0</v>
+        <v>1004</v>
       </c>
       <c r="F20">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G20">
         <v>0</v>
@@ -2118,7 +2129,45 @@
         <v>2</v>
       </c>
       <c r="L20" t="s">
-        <v>67</v>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A21">
+        <v>42</v>
+      </c>
+      <c r="B21" t="s">
+        <v>68</v>
+      </c>
+      <c r="C21" t="s">
+        <v>69</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="J21">
+        <v>0</v>
+      </c>
+      <c r="K21">
+        <v>2</v>
+      </c>
+      <c r="L21" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
init the quest save procedure
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/MainIcon.xlsx
+++ b/ConfigData/Xlsx/MainIcon.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18067"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18229"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Code\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -296,14 +296,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>传记</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>查看自己的传记(T)</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>游戏</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -329,6 +321,14 @@
   </si>
   <si>
     <t>查看我的建造目录</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>任务</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>查看自己的任务(T)</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1375,7 +1375,7 @@
   <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1617,10 +1617,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="C7" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -1731,10 +1731,10 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C10" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -1807,10 +1807,10 @@
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C12" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D12">
         <v>0</v>
@@ -2137,10 +2137,10 @@
         <v>42</v>
       </c>
       <c r="B21" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C21" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D21">
         <v>0</v>
@@ -2167,7 +2167,7 @@
         <v>2</v>
       </c>
       <c r="L21" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix some tooltip show bug
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/MainIcon.xlsx
+++ b/ConfigData/Xlsx/MainIcon.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18229"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,22 +9,22 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
+    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MainIcon" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>real</author>
   </authors>
   <commentList>
-    <comment ref="G2" authorId="0" shapeId="0">
+    <comment ref="G2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -50,7 +50,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H2" authorId="0" shapeId="0">
+    <comment ref="H2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -81,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="73">
   <si>
     <t>打开主菜单(ESC)</t>
   </si>
@@ -156,12 +156,6 @@
   </si>
   <si>
     <t>MapButton2</t>
-  </si>
-  <si>
-    <t>打开锻造系统</t>
-  </si>
-  <si>
-    <t>SideButton1</t>
   </si>
   <si>
     <t>卡片</t>
@@ -335,7 +329,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -531,7 +525,7 @@
       <charset val="134"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -714,6 +708,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -962,7 +962,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -970,6 +970,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1031,21 +1034,21 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:L21" totalsRowShown="0">
-  <autoFilter ref="A1:L21"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="表1" displayName="表1" ref="A1:L20" totalsRowShown="0">
+  <autoFilter ref="A1:L20" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="12">
-    <tableColumn id="1" name="Id"/>
-    <tableColumn id="2" name="Name"/>
-    <tableColumn id="3" name="Des"/>
-    <tableColumn id="4" name="Type"/>
-    <tableColumn id="5" name="Record"/>
-    <tableColumn id="6" name="Level"/>
-    <tableColumn id="7" name="X"/>
-    <tableColumn id="8" name="Y"/>
-    <tableColumn id="9" name="Width"/>
-    <tableColumn id="10" name="Height"/>
-    <tableColumn id="11" name="Flow"/>
-    <tableColumn id="12" name="Icon"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Id"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Name"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Des"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Type"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Record"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Level"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="X"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Y"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Width"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Height"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Flow"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Icon"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1371,11 +1374,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:L20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1389,116 +1392,116 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" t="s">
         <v>53</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>54</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>55</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>56</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>57</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>58</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>59</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>60</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>61</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>62</v>
-      </c>
-      <c r="K1" t="s">
-        <v>63</v>
-      </c>
-      <c r="L1" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="J3" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="K3" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="L3" s="2" t="s">
         <v>50</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.15">
@@ -1617,10 +1620,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C7" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -1731,10 +1734,10 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C10" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -1761,7 +1764,7 @@
         <v>1</v>
       </c>
       <c r="L10" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.15">
@@ -1807,10 +1810,10 @@
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C12" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D12">
         <v>0</v>
@@ -1947,10 +1950,13 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A16">
-        <v>35</v>
+        <v>36</v>
+      </c>
+      <c r="B16" t="s">
+        <v>25</v>
       </c>
       <c r="C16" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D16">
         <v>0</v>
@@ -1959,7 +1965,7 @@
         <v>0</v>
       </c>
       <c r="F16">
-        <v>99</v>
+        <v>20</v>
       </c>
       <c r="G16">
         <v>0</v>
@@ -1977,18 +1983,18 @@
         <v>2</v>
       </c>
       <c r="L16" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A17">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B17" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C17" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D17">
         <v>0</v>
@@ -1996,8 +2002,8 @@
       <c r="E17">
         <v>0</v>
       </c>
-      <c r="F17">
-        <v>20</v>
+      <c r="F17" s="3">
+        <v>50</v>
       </c>
       <c r="G17">
         <v>0</v>
@@ -2015,18 +2021,18 @@
         <v>2</v>
       </c>
       <c r="L17" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A18">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B18" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C18" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D18">
         <v>0</v>
@@ -2034,8 +2040,8 @@
       <c r="E18">
         <v>0</v>
       </c>
-      <c r="F18">
-        <v>99</v>
+      <c r="F18" s="3">
+        <v>50</v>
       </c>
       <c r="G18">
         <v>0</v>
@@ -2053,27 +2059,27 @@
         <v>2</v>
       </c>
       <c r="L18" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A19">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B19" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C19" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E19">
-        <v>0</v>
+        <v>1004</v>
       </c>
       <c r="F19">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="G19">
         <v>0</v>
@@ -2091,27 +2097,27 @@
         <v>2</v>
       </c>
       <c r="L19" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A20">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B20" t="s">
-        <v>36</v>
+        <v>64</v>
       </c>
       <c r="C20" t="s">
-        <v>37</v>
+        <v>65</v>
       </c>
       <c r="D20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E20">
-        <v>1004</v>
-      </c>
-      <c r="F20">
-        <v>20</v>
+        <v>0</v>
+      </c>
+      <c r="F20" s="3">
+        <v>50</v>
       </c>
       <c r="G20">
         <v>0</v>
@@ -2129,45 +2135,7 @@
         <v>2</v>
       </c>
       <c r="L20" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A21">
-        <v>42</v>
-      </c>
-      <c r="B21" t="s">
         <v>66</v>
-      </c>
-      <c r="C21" t="s">
-        <v>67</v>
-      </c>
-      <c r="D21">
-        <v>0</v>
-      </c>
-      <c r="E21">
-        <v>0</v>
-      </c>
-      <c r="F21">
-        <v>0</v>
-      </c>
-      <c r="G21">
-        <v>0</v>
-      </c>
-      <c r="H21">
-        <v>0</v>
-      </c>
-      <c r="I21">
-        <v>0</v>
-      </c>
-      <c r="J21">
-        <v>0</v>
-      </c>
-      <c r="K21">
-        <v>2</v>
-      </c>
-      <c r="L21" t="s">
-        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
let the dailycard refresh every day
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/MainIcon.xlsx
+++ b/ConfigData/Xlsx/MainIcon.xlsx
@@ -164,177 +164,178 @@
     <t>打开卡片商店面板</t>
   </si>
   <si>
+    <t>锦标</t>
+  </si>
+  <si>
+    <t>打开赛事锦标</t>
+  </si>
+  <si>
+    <t>SideButton5</t>
+  </si>
+  <si>
+    <t>转盘</t>
+  </si>
+  <si>
+    <t>打开幸运转盘界面</t>
+  </si>
+  <si>
+    <t>SideButton16</t>
+  </si>
+  <si>
+    <t>问答</t>
+  </si>
+  <si>
+    <t>打开问答界面</t>
+  </si>
+  <si>
+    <t>SideButton7</t>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>序列</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>名字</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>描述</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>分类</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>对应记录</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>开放等级</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>绝对坐标x</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>绝对坐标y</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>宽度</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>高度</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>所属位置流</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>路径</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Id</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Des</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Record</t>
+  </si>
+  <si>
+    <t>Level</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Width</t>
+  </si>
+  <si>
+    <t>Height</t>
+  </si>
+  <si>
+    <t>Flow</t>
+  </si>
+  <si>
+    <t>Icon</t>
+  </si>
+  <si>
+    <t>MainIcon10</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>游戏</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>打开迷你游戏面板</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>城堡</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>查看城堡的状态(C)</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>建造</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>查看我的建造目录</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>任务</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>查看自己的任务(T)</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>SideButton4</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>合成</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>打开每日合成卡牌</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>SideButton2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
     <t>SideButton9</t>
-  </si>
-  <si>
-    <t>锦标</t>
-  </si>
-  <si>
-    <t>打开赛事锦标</t>
-  </si>
-  <si>
-    <t>SideButton5</t>
-  </si>
-  <si>
-    <t>转盘</t>
-  </si>
-  <si>
-    <t>打开幸运转盘界面</t>
-  </si>
-  <si>
-    <t>SideButton16</t>
-  </si>
-  <si>
-    <t>问答</t>
-  </si>
-  <si>
-    <t>打开问答界面</t>
-  </si>
-  <si>
-    <t>SideButton7</t>
-  </si>
-  <si>
-    <t>int</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>string</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>序列</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>名字</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>描述</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>分类</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>对应记录</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>开放等级</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>绝对坐标x</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>绝对坐标y</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>宽度</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>高度</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>所属位置流</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>路径</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Id</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Des</t>
-  </si>
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t>Record</t>
-  </si>
-  <si>
-    <t>Level</t>
-  </si>
-  <si>
-    <t>X</t>
-  </si>
-  <si>
-    <t>Y</t>
-  </si>
-  <si>
-    <t>Width</t>
-  </si>
-  <si>
-    <t>Height</t>
-  </si>
-  <si>
-    <t>Flow</t>
-  </si>
-  <si>
-    <t>Icon</t>
-  </si>
-  <si>
-    <t>MainIcon10</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>游戏</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>打开迷你游戏面板</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>城堡</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>查看城堡的状态(C)</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>建造</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>查看我的建造目录</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>任务</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>查看自己的任务(T)</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>SideButton4</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>合成</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>打开每日合成卡牌</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>SideButton2</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1390,7 +1391,7 @@
   <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1404,116 +1405,116 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" t="s">
         <v>51</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>52</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>53</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>54</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>55</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>56</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>57</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>58</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>59</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>60</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>61</v>
-      </c>
-      <c r="L1" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>38</v>
-      </c>
       <c r="C2" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="L2" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="J3" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="K3" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="L3" s="2" t="s">
         <v>49</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.15">
@@ -1632,10 +1633,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>69</v>
+      </c>
+      <c r="C7" t="s">
         <v>70</v>
-      </c>
-      <c r="C7" t="s">
-        <v>71</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -1746,10 +1747,10 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
+        <v>67</v>
+      </c>
+      <c r="C10" t="s">
         <v>68</v>
-      </c>
-      <c r="C10" t="s">
-        <v>69</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -1776,7 +1777,7 @@
         <v>1</v>
       </c>
       <c r="L10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.15">
@@ -1822,10 +1823,10 @@
         <v>12</v>
       </c>
       <c r="B12" t="s">
+        <v>65</v>
+      </c>
+      <c r="C12" t="s">
         <v>66</v>
-      </c>
-      <c r="C12" t="s">
-        <v>67</v>
       </c>
       <c r="D12">
         <v>0</v>
@@ -1995,7 +1996,7 @@
         <v>2</v>
       </c>
       <c r="L16" t="s">
-        <v>27</v>
+        <v>74</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.15">
@@ -2003,10 +2004,10 @@
         <v>37</v>
       </c>
       <c r="B17" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" t="s">
         <v>28</v>
-      </c>
-      <c r="C17" t="s">
-        <v>29</v>
       </c>
       <c r="D17">
         <v>0</v>
@@ -2033,7 +2034,7 @@
         <v>2</v>
       </c>
       <c r="L17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.15">
@@ -2041,10 +2042,10 @@
         <v>39</v>
       </c>
       <c r="B18" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" t="s">
         <v>31</v>
-      </c>
-      <c r="C18" t="s">
-        <v>32</v>
       </c>
       <c r="D18">
         <v>0</v>
@@ -2071,7 +2072,7 @@
         <v>2</v>
       </c>
       <c r="L18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.15">
@@ -2079,10 +2080,10 @@
         <v>40</v>
       </c>
       <c r="B19" t="s">
+        <v>72</v>
+      </c>
+      <c r="C19" t="s">
         <v>73</v>
-      </c>
-      <c r="C19" t="s">
-        <v>74</v>
       </c>
       <c r="D19">
         <v>0</v>
@@ -2117,10 +2118,10 @@
         <v>41</v>
       </c>
       <c r="B20" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20" t="s">
         <v>34</v>
-      </c>
-      <c r="C20" t="s">
-        <v>35</v>
       </c>
       <c r="D20">
         <v>1</v>
@@ -2147,7 +2148,7 @@
         <v>2</v>
       </c>
       <c r="L20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.15">
@@ -2155,10 +2156,10 @@
         <v>42</v>
       </c>
       <c r="B21" t="s">
+        <v>63</v>
+      </c>
+      <c r="C21" t="s">
         <v>64</v>
-      </c>
-      <c r="C21" t="s">
-        <v>65</v>
       </c>
       <c r="D21">
         <v>0</v>
@@ -2185,7 +2186,7 @@
         <v>2</v>
       </c>
       <c r="L21" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
dungeon deck select system almost finish
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/MainIcon.xlsx
+++ b/ConfigData/Xlsx/MainIcon.xlsx
@@ -1445,7 +1445,7 @@
   <dimension ref="A1:N22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1743,7 +1743,7 @@
         <v>79</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I7">
         <v>0</v>
@@ -1787,7 +1787,7 @@
         <v>79</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I8">
         <v>0</v>
@@ -1828,7 +1828,7 @@
         <v>2</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H9" s="5" t="s">
         <v>79</v>

</xml_diff>

<commit_message>
add a dungeon card event
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/MainIcon.xlsx
+++ b/ConfigData/Xlsx/MainIcon.xlsx
@@ -81,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="86">
   <si>
     <t>打开主菜单(ESC)</t>
   </si>
@@ -358,11 +358,15 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>查看我的卡组(D)</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>MainIcon6</t>
+  </si>
+  <si>
+    <t>查看我的副本定制卡组(D)</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>定制</t>
+    <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1445,7 +1449,7 @@
   <dimension ref="A1:N22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="H17" sqref="H17:H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1813,10 +1817,10 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>85</v>
       </c>
       <c r="C9" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -1849,7 +1853,7 @@
         <v>1</v>
       </c>
       <c r="N9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.15">
@@ -1875,7 +1879,7 @@
         <v>79</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I10">
         <v>0</v>
@@ -2174,7 +2178,7 @@
         <v>79</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I17">
         <v>0</v>
@@ -2218,7 +2222,7 @@
         <v>79</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I18">
         <v>0</v>
@@ -2262,7 +2266,7 @@
         <v>79</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I19">
         <v>0</v>
@@ -2306,7 +2310,7 @@
         <v>79</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I20">
         <v>0</v>
@@ -2350,7 +2354,7 @@
         <v>79</v>
       </c>
       <c r="H21" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I21">
         <v>0</v>
@@ -2394,7 +2398,7 @@
         <v>79</v>
       </c>
       <c r="H22" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I22">
         <v>0</v>

</xml_diff>

<commit_message>
add the story form
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/MainIcon.xlsx
+++ b/ConfigData/Xlsx/MainIcon.xlsx
@@ -81,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="88">
   <si>
     <t>打开主菜单(ESC)</t>
   </si>
@@ -366,6 +366,14 @@
   </si>
   <si>
     <t>定制</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>故事</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>打开副本故事面板</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1103,8 +1111,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:N22" totalsRowShown="0" headerRowDxfId="2">
-  <autoFilter ref="A1:N22"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:N23" totalsRowShown="0" headerRowDxfId="2">
+  <autoFilter ref="A1:N23"/>
   <tableColumns count="14">
     <tableColumn id="1" name="序列"/>
     <tableColumn id="2" name="名字"/>
@@ -1446,10 +1454,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N22"/>
+  <dimension ref="A1:N23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17:H22"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2419,6 +2427,50 @@
         <v>56</v>
       </c>
     </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A23">
+        <v>43</v>
+      </c>
+      <c r="B23" t="s">
+        <v>86</v>
+      </c>
+      <c r="C23" t="s">
+        <v>87</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="H23" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="I23">
+        <v>0</v>
+      </c>
+      <c r="J23">
+        <v>0</v>
+      </c>
+      <c r="K23">
+        <v>0</v>
+      </c>
+      <c r="L23">
+        <v>0</v>
+      </c>
+      <c r="M23">
+        <v>2</v>
+      </c>
+      <c r="N23" t="s">
+        <v>59</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add a user form to show user records
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/MainIcon.xlsx
+++ b/ConfigData/Xlsx/MainIcon.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19001"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\code\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TOMClassic\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -81,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="92">
   <si>
     <t>打开主菜单(ESC)</t>
   </si>
@@ -98,286 +98,299 @@
     <t>MainIcon8</t>
   </si>
   <si>
+    <t>挑战</t>
+  </si>
+  <si>
+    <t>挑战自己结识的对手(F)</t>
+  </si>
+  <si>
+    <t>MainIcon5</t>
+  </si>
+  <si>
+    <t>卡组</t>
+  </si>
+  <si>
+    <t>编辑我的卡组(D)</t>
+  </si>
+  <si>
+    <t>MainIcon7</t>
+  </si>
+  <si>
+    <t>物品</t>
+  </si>
+  <si>
+    <t>查看我的物品(I)</t>
+  </si>
+  <si>
+    <t>MainIcon2</t>
+  </si>
+  <si>
+    <t>MainIcon4</t>
+  </si>
+  <si>
+    <t>打开魔法书</t>
+  </si>
+  <si>
+    <t>MapButton3</t>
+  </si>
+  <si>
+    <t>打开世界地图(M)</t>
+  </si>
+  <si>
+    <t>MapButton1</t>
+  </si>
+  <si>
+    <t>反馈信息</t>
+  </si>
+  <si>
+    <t>MapButton2</t>
+  </si>
+  <si>
+    <t>卡片</t>
+  </si>
+  <si>
+    <t>打开卡片商店面板</t>
+  </si>
+  <si>
+    <t>锦标</t>
+  </si>
+  <si>
+    <t>打开赛事锦标</t>
+  </si>
+  <si>
+    <t>SideButton5</t>
+  </si>
+  <si>
+    <t>转盘</t>
+  </si>
+  <si>
+    <t>打开幸运转盘界面</t>
+  </si>
+  <si>
+    <t>SideButton16</t>
+  </si>
+  <si>
+    <t>问答</t>
+  </si>
+  <si>
+    <t>打开问答界面</t>
+  </si>
+  <si>
+    <t>SideButton7</t>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Id</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Des</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Record</t>
+  </si>
+  <si>
+    <t>Level</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Width</t>
+  </si>
+  <si>
+    <t>Height</t>
+  </si>
+  <si>
+    <t>Flow</t>
+  </si>
+  <si>
+    <t>Icon</t>
+  </si>
+  <si>
+    <t>MainIcon10</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>游戏</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>打开迷你游戏面板</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>城堡</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>查看城堡的状态(C)</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>建造</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>查看我的建造目录</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>任务</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>查看自己的任务(T)</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>SideButton4</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>合成</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>打开每日合成卡牌</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>SideButton2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>SideButton9</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>序列</t>
+  </si>
+  <si>
+    <t>名字</t>
+  </si>
+  <si>
+    <t>描述</t>
+  </si>
+  <si>
+    <t>分类</t>
+  </si>
+  <si>
+    <t>对应记录</t>
+  </si>
+  <si>
+    <t>开放等级</t>
+  </si>
+  <si>
+    <t>绝对坐标x</t>
+  </si>
+  <si>
+    <t>绝对坐标y</t>
+  </si>
+  <si>
+    <t>宽度</t>
+  </si>
+  <si>
+    <t>高度</t>
+  </si>
+  <si>
+    <t>所属位置流</t>
+  </si>
+  <si>
+    <t>路径</t>
+  </si>
+  <si>
+    <t>副本中显示</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>场景中显示</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>bool</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>ShowInScene</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>ShowInDungeon</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>false</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>true</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>离开</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>离开副本</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>SideButton6</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>MainIcon6</t>
+  </si>
+  <si>
+    <t>查看我的副本定制卡组(D)</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>定制</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>故事</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>打开副本故事面板</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>SideButton3</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>传记</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>进入传记</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
     <t>MainIcon3</t>
-  </si>
-  <si>
-    <t>挑战</t>
-  </si>
-  <si>
-    <t>挑战自己结识的对手(F)</t>
-  </si>
-  <si>
-    <t>MainIcon5</t>
-  </si>
-  <si>
-    <t>卡组</t>
-  </si>
-  <si>
-    <t>编辑我的卡组(D)</t>
-  </si>
-  <si>
-    <t>MainIcon7</t>
-  </si>
-  <si>
-    <t>物品</t>
-  </si>
-  <si>
-    <t>查看我的物品(I)</t>
-  </si>
-  <si>
-    <t>MainIcon2</t>
-  </si>
-  <si>
-    <t>MainIcon4</t>
-  </si>
-  <si>
-    <t>打开魔法书</t>
-  </si>
-  <si>
-    <t>MapButton3</t>
-  </si>
-  <si>
-    <t>打开世界地图(M)</t>
-  </si>
-  <si>
-    <t>MapButton1</t>
-  </si>
-  <si>
-    <t>反馈信息</t>
-  </si>
-  <si>
-    <t>MapButton2</t>
-  </si>
-  <si>
-    <t>卡片</t>
-  </si>
-  <si>
-    <t>打开卡片商店面板</t>
-  </si>
-  <si>
-    <t>锦标</t>
-  </si>
-  <si>
-    <t>打开赛事锦标</t>
-  </si>
-  <si>
-    <t>SideButton5</t>
-  </si>
-  <si>
-    <t>转盘</t>
-  </si>
-  <si>
-    <t>打开幸运转盘界面</t>
-  </si>
-  <si>
-    <t>SideButton16</t>
-  </si>
-  <si>
-    <t>问答</t>
-  </si>
-  <si>
-    <t>打开问答界面</t>
-  </si>
-  <si>
-    <t>SideButton7</t>
-  </si>
-  <si>
-    <t>int</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>string</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Id</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Des</t>
-  </si>
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t>Record</t>
-  </si>
-  <si>
-    <t>Level</t>
-  </si>
-  <si>
-    <t>X</t>
-  </si>
-  <si>
-    <t>Y</t>
-  </si>
-  <si>
-    <t>Width</t>
-  </si>
-  <si>
-    <t>Height</t>
-  </si>
-  <si>
-    <t>Flow</t>
-  </si>
-  <si>
-    <t>Icon</t>
-  </si>
-  <si>
-    <t>MainIcon10</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>游戏</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>打开迷你游戏面板</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>城堡</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>查看城堡的状态(C)</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>建造</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>查看我的建造目录</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>任务</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>查看自己的任务(T)</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>SideButton4</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>合成</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>打开每日合成卡牌</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>SideButton2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>SideButton9</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>序列</t>
-  </si>
-  <si>
-    <t>名字</t>
-  </si>
-  <si>
-    <t>描述</t>
-  </si>
-  <si>
-    <t>分类</t>
-  </si>
-  <si>
-    <t>对应记录</t>
-  </si>
-  <si>
-    <t>开放等级</t>
-  </si>
-  <si>
-    <t>绝对坐标x</t>
-  </si>
-  <si>
-    <t>绝对坐标y</t>
-  </si>
-  <si>
-    <t>宽度</t>
-  </si>
-  <si>
-    <t>高度</t>
-  </si>
-  <si>
-    <t>所属位置流</t>
-  </si>
-  <si>
-    <t>路径</t>
-  </si>
-  <si>
-    <t>副本中显示</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>场景中显示</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>bool</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>ShowInScene</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>ShowInDungeon</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>false</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>true</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>离开</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>离开副本</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>SideButton6</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>MainIcon6</t>
-  </si>
-  <si>
-    <t>查看我的副本定制卡组(D)</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>定制</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>故事</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>打开副本故事面板</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>SideButton3</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>MainIcon9</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1115,8 +1128,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:N23" totalsRowShown="0" headerRowDxfId="2">
-  <autoFilter ref="A1:N23"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:N24" totalsRowShown="0" headerRowDxfId="2">
+  <autoFilter ref="A1:N24"/>
   <tableColumns count="14">
     <tableColumn id="1" name="序列"/>
     <tableColumn id="2" name="名字"/>
@@ -1458,10 +1471,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N23"/>
+  <dimension ref="A1:N24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N18" sqref="N18"/>
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1477,134 +1490,134 @@
   <sheetData>
     <row r="1" spans="1:14" ht="57" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="I1" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="G1" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>71</v>
-      </c>
-      <c r="N1" s="4" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>34</v>
-      </c>
       <c r="C2" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="N2" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="I3" s="2" t="s">
+      <c r="J3" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="K3" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="L3" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="L3" s="2" t="s">
+      <c r="M3" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="M3" s="2" t="s">
+      <c r="N3" s="2" t="s">
         <v>45</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.15">
@@ -1624,10 +1637,10 @@
         <v>0</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I4">
         <v>-82</v>
@@ -1668,10 +1681,10 @@
         <v>10</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I5">
         <v>0</v>
@@ -1694,13 +1707,13 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A6">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>54</v>
+        <v>88</v>
       </c>
       <c r="C6" t="s">
-        <v>55</v>
+        <v>89</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -1712,10 +1725,10 @@
         <v>0</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I6">
         <v>0</v>
@@ -1733,18 +1746,18 @@
         <v>1</v>
       </c>
       <c r="N6" t="s">
-        <v>5</v>
+        <v>91</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A7">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>53</v>
       </c>
       <c r="C7" t="s">
-        <v>7</v>
+        <v>54</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -1753,10 +1766,10 @@
         <v>0</v>
       </c>
       <c r="F7">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H7" s="5" t="s">
         <v>78</v>
@@ -1777,18 +1790,18 @@
         <v>1</v>
       </c>
       <c r="N7" t="s">
-        <v>8</v>
+        <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A8">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -1797,13 +1810,13 @@
         <v>0</v>
       </c>
       <c r="F8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I8">
         <v>0</v>
@@ -1821,18 +1834,18 @@
         <v>1</v>
       </c>
       <c r="N8" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" t="s">
         <v>9</v>
-      </c>
-      <c r="B9" t="s">
-        <v>85</v>
-      </c>
-      <c r="C9" t="s">
-        <v>84</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -1847,7 +1860,7 @@
         <v>78</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="I9">
         <v>0</v>
@@ -1865,18 +1878,18 @@
         <v>1</v>
       </c>
       <c r="N9" t="s">
-        <v>83</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A10">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>52</v>
+        <v>84</v>
       </c>
       <c r="C10" t="s">
-        <v>53</v>
+        <v>83</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -1885,10 +1898,10 @@
         <v>0</v>
       </c>
       <c r="F10">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H10" s="5" t="s">
         <v>78</v>
@@ -1909,18 +1922,18 @@
         <v>1</v>
       </c>
       <c r="N10" t="s">
-        <v>47</v>
+        <v>82</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A11">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>12</v>
+        <v>51</v>
       </c>
       <c r="C11" t="s">
-        <v>13</v>
+        <v>52</v>
       </c>
       <c r="D11">
         <v>0</v>
@@ -1929,13 +1942,13 @@
         <v>0</v>
       </c>
       <c r="F11">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="I11">
         <v>0</v>
@@ -1953,19 +1966,19 @@
         <v>1</v>
       </c>
       <c r="N11" t="s">
-        <v>14</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" t="s">
         <v>12</v>
       </c>
-      <c r="B12" t="s">
-        <v>50</v>
-      </c>
-      <c r="C12" t="s">
-        <v>51</v>
-      </c>
       <c r="D12">
         <v>0</v>
       </c>
@@ -1976,10 +1989,10 @@
         <v>0</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I12">
         <v>0</v>
@@ -1997,18 +2010,18 @@
         <v>1</v>
       </c>
       <c r="N12" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A13">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>80</v>
+        <v>49</v>
       </c>
       <c r="C13" t="s">
-        <v>81</v>
+        <v>50</v>
       </c>
       <c r="D13">
         <v>0</v>
@@ -2023,33 +2036,36 @@
         <v>78</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I13">
-        <v>-60</v>
+        <v>0</v>
       </c>
       <c r="J13">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="K13">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="L13">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="M13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N13" t="s">
-        <v>82</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A14">
-        <v>32</v>
+        <v>31</v>
+      </c>
+      <c r="B14" t="s">
+        <v>79</v>
       </c>
       <c r="C14" t="s">
-        <v>16</v>
+        <v>80</v>
       </c>
       <c r="D14">
         <v>0</v>
@@ -2061,36 +2077,36 @@
         <v>0</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H14" s="5" t="s">
         <v>78</v>
       </c>
       <c r="I14">
-        <v>-184</v>
+        <v>-60</v>
       </c>
       <c r="J14">
-        <v>120</v>
+        <v>60</v>
       </c>
       <c r="K14">
-        <v>28</v>
+        <v>50</v>
       </c>
       <c r="L14">
-        <v>28</v>
+        <v>50</v>
       </c>
       <c r="M14">
         <v>0</v>
       </c>
       <c r="N14" t="s">
-        <v>17</v>
+        <v>81</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A15">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C15" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D15">
         <v>0</v>
@@ -2102,36 +2118,36 @@
         <v>0</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I15">
         <v>-184</v>
       </c>
       <c r="J15">
-        <v>62</v>
+        <v>120</v>
       </c>
       <c r="K15">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="L15">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="M15">
         <v>0</v>
       </c>
       <c r="N15" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A16">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C16" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D16">
         <v>0</v>
@@ -2143,39 +2159,36 @@
         <v>0</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I16">
         <v>-184</v>
       </c>
       <c r="J16">
-        <v>155</v>
+        <v>62</v>
       </c>
       <c r="K16">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="L16">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="M16">
         <v>0</v>
       </c>
       <c r="N16" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A17">
-        <v>36</v>
-      </c>
-      <c r="B17" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="C17" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D17">
         <v>0</v>
@@ -2184,42 +2197,42 @@
         <v>0</v>
       </c>
       <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="I17">
+        <v>-184</v>
+      </c>
+      <c r="J17">
+        <v>155</v>
+      </c>
+      <c r="K17">
+        <v>28</v>
+      </c>
+      <c r="L17">
+        <v>28</v>
+      </c>
+      <c r="M17">
+        <v>0</v>
+      </c>
+      <c r="N17" t="s">
         <v>20</v>
-      </c>
-      <c r="G17" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="H17" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="I17">
-        <v>0</v>
-      </c>
-      <c r="J17">
-        <v>0</v>
-      </c>
-      <c r="K17">
-        <v>0</v>
-      </c>
-      <c r="L17">
-        <v>0</v>
-      </c>
-      <c r="M17">
-        <v>2</v>
-      </c>
-      <c r="N17" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A18">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B18" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C18" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D18">
         <v>0</v>
@@ -2227,14 +2240,14 @@
       <c r="E18">
         <v>0</v>
       </c>
-      <c r="F18" s="3">
-        <v>50</v>
+      <c r="F18">
+        <v>20</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I18">
         <v>0</v>
@@ -2252,18 +2265,18 @@
         <v>2</v>
       </c>
       <c r="N18" t="s">
-        <v>26</v>
+        <v>87</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A19">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B19" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C19" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D19">
         <v>0</v>
@@ -2275,10 +2288,10 @@
         <v>50</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I19">
         <v>0</v>
@@ -2296,18 +2309,18 @@
         <v>2</v>
       </c>
       <c r="N19" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A20">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B20" t="s">
-        <v>57</v>
+        <v>26</v>
       </c>
       <c r="C20" t="s">
-        <v>58</v>
+        <v>27</v>
       </c>
       <c r="D20">
         <v>0</v>
@@ -2315,14 +2328,14 @@
       <c r="E20">
         <v>0</v>
       </c>
-      <c r="F20">
-        <v>5</v>
+      <c r="F20" s="3">
+        <v>50</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I20">
         <v>0</v>
@@ -2340,33 +2353,33 @@
         <v>2</v>
       </c>
       <c r="N20" t="s">
-        <v>60</v>
+        <v>28</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A21">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B21" t="s">
-        <v>30</v>
+        <v>56</v>
       </c>
       <c r="C21" t="s">
-        <v>31</v>
+        <v>57</v>
       </c>
       <c r="D21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E21">
-        <v>1004</v>
+        <v>0</v>
       </c>
       <c r="F21">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H21" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I21">
         <v>0</v>
@@ -2384,33 +2397,33 @@
         <v>2</v>
       </c>
       <c r="N21" t="s">
-        <v>32</v>
+        <v>59</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A22">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B22" t="s">
-        <v>48</v>
+        <v>29</v>
       </c>
       <c r="C22" t="s">
-        <v>49</v>
+        <v>30</v>
       </c>
       <c r="D22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E22">
-        <v>0</v>
-      </c>
-      <c r="F22" s="3">
-        <v>50</v>
+        <v>1004</v>
+      </c>
+      <c r="F22">
+        <v>20</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H22" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I22">
         <v>0</v>
@@ -2428,18 +2441,18 @@
         <v>2</v>
       </c>
       <c r="N22" t="s">
-        <v>56</v>
+        <v>31</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A23">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B23" t="s">
-        <v>86</v>
+        <v>47</v>
       </c>
       <c r="C23" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="D23">
         <v>0</v>
@@ -2447,14 +2460,14 @@
       <c r="E23">
         <v>0</v>
       </c>
-      <c r="F23">
-        <v>0</v>
+      <c r="F23" s="3">
+        <v>50</v>
       </c>
       <c r="G23" s="5" t="s">
         <v>78</v>
       </c>
       <c r="H23" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="I23">
         <v>0</v>
@@ -2472,7 +2485,51 @@
         <v>2</v>
       </c>
       <c r="N23" t="s">
-        <v>59</v>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A24">
+        <v>43</v>
+      </c>
+      <c r="B24" t="s">
+        <v>85</v>
+      </c>
+      <c r="C24" t="s">
+        <v>86</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="H24" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="I24">
+        <v>0</v>
+      </c>
+      <c r="J24">
+        <v>0</v>
+      </c>
+      <c r="K24">
+        <v>0</v>
+      </c>
+      <c r="L24">
+        <v>0</v>
+      </c>
+      <c r="M24">
+        <v>2</v>
+      </c>
+      <c r="N24" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finish the rank system
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/MainIcon.xlsx
+++ b/ConfigData/Xlsx/MainIcon.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19029"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Code\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -92,36 +92,24 @@
     <t>商城</t>
   </si>
   <si>
-    <t>进入商城(V)</t>
-  </si>
-  <si>
     <t>MainIcon8</t>
   </si>
   <si>
     <t>挑战</t>
   </si>
   <si>
-    <t>挑战自己结识的对手(F)</t>
-  </si>
-  <si>
     <t>MainIcon5</t>
   </si>
   <si>
     <t>卡组</t>
   </si>
   <si>
-    <t>编辑我的卡组(D)</t>
-  </si>
-  <si>
     <t>MainIcon7</t>
   </si>
   <si>
     <t>物品</t>
   </si>
   <si>
-    <t>查看我的物品(I)</t>
-  </si>
-  <si>
     <t>MainIcon2</t>
   </si>
   <si>
@@ -134,15 +122,9 @@
     <t>MapButton3</t>
   </si>
   <si>
-    <t>打开世界地图(M)</t>
-  </si>
-  <si>
     <t>MapButton1</t>
   </si>
   <si>
-    <t>反馈信息</t>
-  </si>
-  <si>
     <t>MapButton2</t>
   </si>
   <si>
@@ -239,10 +221,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>查看城堡的状态(C)</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>建造</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -255,10 +233,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>查看自己的任务(T)</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>SideButton4</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -358,10 +332,6 @@
     <t>MainIcon6</t>
   </si>
   <si>
-    <t>查看我的副本定制卡组(D)</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>定制</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -391,6 +361,42 @@
   </si>
   <si>
     <t>MainIcon9</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>排行榜</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>打开世界地图</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>查看城堡的状态</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>查看我的物品</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>查看我的副本定制卡组</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>编辑我的卡组</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>挑战自己结识的对手</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>查看自己的任务</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>进入商城</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1116,74 +1122,6 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1226,7 +1164,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="C7EDCC"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -1542,7 +1480,7 @@
   <dimension ref="A1:N24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1558,134 +1496,134 @@
   <sheetData>
     <row r="1" spans="1:14" ht="57" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="K1" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>63</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="N1" s="4" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="J3" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="K3" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="L3" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="M3" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="N3" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.15">
@@ -1705,10 +1643,10 @@
         <v>0</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="I4">
         <v>-82</v>
@@ -1737,7 +1675,7 @@
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>3</v>
+        <v>91</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -1749,10 +1687,10 @@
         <v>10</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="I5">
         <v>0</v>
@@ -1770,7 +1708,7 @@
         <v>1</v>
       </c>
       <c r="N5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.15">
@@ -1778,10 +1716,10 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="C6" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -1793,10 +1731,10 @@
         <v>0</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="I6">
         <v>0</v>
@@ -1814,7 +1752,7 @@
         <v>1</v>
       </c>
       <c r="N6" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.15">
@@ -1822,10 +1760,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="C7" t="s">
-        <v>54</v>
+        <v>90</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -1837,10 +1775,10 @@
         <v>0</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="I7">
         <v>0</v>
@@ -1858,7 +1796,7 @@
         <v>1</v>
       </c>
       <c r="N7" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.15">
@@ -1866,10 +1804,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>6</v>
+        <v>89</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -1881,10 +1819,10 @@
         <v>3</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="I8">
         <v>0</v>
@@ -1902,7 +1840,7 @@
         <v>1</v>
       </c>
       <c r="N8" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.15">
@@ -1910,10 +1848,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>9</v>
+        <v>88</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -1925,10 +1863,10 @@
         <v>2</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="I9">
         <v>0</v>
@@ -1946,7 +1884,7 @@
         <v>1</v>
       </c>
       <c r="N9" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.15">
@@ -1954,10 +1892,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="C10" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -1969,10 +1907,10 @@
         <v>2</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="I10">
         <v>0</v>
@@ -1990,7 +1928,7 @@
         <v>1</v>
       </c>
       <c r="N10" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.15">
@@ -1998,10 +1936,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="C11" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="D11">
         <v>0</v>
@@ -2013,10 +1951,10 @@
         <v>7</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="I11">
         <v>0</v>
@@ -2034,7 +1972,7 @@
         <v>1</v>
       </c>
       <c r="N11" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.15">
@@ -2042,10 +1980,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C12" t="s">
-        <v>12</v>
+        <v>86</v>
       </c>
       <c r="D12">
         <v>0</v>
@@ -2057,10 +1995,10 @@
         <v>0</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="I12">
         <v>0</v>
@@ -2078,7 +2016,7 @@
         <v>1</v>
       </c>
       <c r="N12" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.15">
@@ -2086,10 +2024,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C13" t="s">
-        <v>50</v>
+        <v>85</v>
       </c>
       <c r="D13">
         <v>0</v>
@@ -2101,10 +2039,10 @@
         <v>0</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="I13">
         <v>0</v>
@@ -2122,7 +2060,7 @@
         <v>1</v>
       </c>
       <c r="N13" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.15">
@@ -2130,10 +2068,10 @@
         <v>31</v>
       </c>
       <c r="B14" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="C14" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="D14">
         <v>0</v>
@@ -2145,10 +2083,10 @@
         <v>0</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="I14">
         <v>-60</v>
@@ -2166,7 +2104,7 @@
         <v>0</v>
       </c>
       <c r="N14" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.15">
@@ -2174,7 +2112,7 @@
         <v>32</v>
       </c>
       <c r="C15" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D15">
         <v>0</v>
@@ -2186,10 +2124,10 @@
         <v>0</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="I15">
         <v>-184</v>
@@ -2207,7 +2145,7 @@
         <v>0</v>
       </c>
       <c r="N15" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.15">
@@ -2215,7 +2153,7 @@
         <v>33</v>
       </c>
       <c r="C16" t="s">
-        <v>17</v>
+        <v>84</v>
       </c>
       <c r="D16">
         <v>0</v>
@@ -2227,10 +2165,10 @@
         <v>0</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="I16">
         <v>-184</v>
@@ -2248,7 +2186,7 @@
         <v>0</v>
       </c>
       <c r="N16" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.15">
@@ -2256,7 +2194,7 @@
         <v>34</v>
       </c>
       <c r="C17" t="s">
-        <v>19</v>
+        <v>83</v>
       </c>
       <c r="D17">
         <v>0</v>
@@ -2265,13 +2203,13 @@
         <v>0</v>
       </c>
       <c r="F17">
-        <v>99</v>
+        <v>0</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="I17">
         <v>-184</v>
@@ -2289,7 +2227,7 @@
         <v>0</v>
       </c>
       <c r="N17" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.15">
@@ -2297,10 +2235,10 @@
         <v>36</v>
       </c>
       <c r="B18" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C18" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D18">
         <v>0</v>
@@ -2312,10 +2250,10 @@
         <v>20</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="I18">
         <v>0</v>
@@ -2333,7 +2271,7 @@
         <v>2</v>
       </c>
       <c r="N18" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.15">
@@ -2341,10 +2279,10 @@
         <v>37</v>
       </c>
       <c r="B19" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C19" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="D19">
         <v>0</v>
@@ -2356,10 +2294,10 @@
         <v>50</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="I19">
         <v>0</v>
@@ -2377,7 +2315,7 @@
         <v>2</v>
       </c>
       <c r="N19" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.15">
@@ -2385,10 +2323,10 @@
         <v>39</v>
       </c>
       <c r="B20" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C20" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D20">
         <v>0</v>
@@ -2400,10 +2338,10 @@
         <v>50</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="I20">
         <v>0</v>
@@ -2421,7 +2359,7 @@
         <v>2</v>
       </c>
       <c r="N20" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.15">
@@ -2429,10 +2367,10 @@
         <v>40</v>
       </c>
       <c r="B21" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="C21" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="D21">
         <v>0</v>
@@ -2444,10 +2382,10 @@
         <v>5</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="H21" s="5" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="I21">
         <v>0</v>
@@ -2465,7 +2403,7 @@
         <v>2</v>
       </c>
       <c r="N21" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.15">
@@ -2473,10 +2411,10 @@
         <v>41</v>
       </c>
       <c r="B22" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C22" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D22">
         <v>1</v>
@@ -2488,10 +2426,10 @@
         <v>20</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="H22" s="5" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="I22">
         <v>0</v>
@@ -2509,7 +2447,7 @@
         <v>2</v>
       </c>
       <c r="N22" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.15">
@@ -2517,10 +2455,10 @@
         <v>42</v>
       </c>
       <c r="B23" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="C23" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D23">
         <v>0</v>
@@ -2532,10 +2470,10 @@
         <v>50</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="H23" s="5" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="I23">
         <v>0</v>
@@ -2553,7 +2491,7 @@
         <v>2</v>
       </c>
       <c r="N23" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.15">
@@ -2561,10 +2499,10 @@
         <v>43</v>
       </c>
       <c r="B24" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="C24" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="D24">
         <v>0</v>
@@ -2576,10 +2514,10 @@
         <v>0</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="H24" s="5" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="I24">
         <v>0</v>
@@ -2597,7 +2535,7 @@
         <v>2</v>
       </c>
       <c r="N24" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add a role form
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/MainIcon.xlsx
+++ b/ConfigData/Xlsx/MainIcon.xlsx
@@ -81,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="92">
   <si>
     <t>打开主菜单(ESC)</t>
   </si>
@@ -386,6 +386,17 @@
   <si>
     <t>进入商城</t>
     <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>角色</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>进入自己的角色</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>MainIcon10</t>
   </si>
 </sst>
 </file>
@@ -1122,8 +1133,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:N23" totalsRowShown="0" headerRowDxfId="2">
-  <autoFilter ref="A1:N23"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:N24" totalsRowShown="0" headerRowDxfId="2">
+  <autoFilter ref="A1:N24"/>
   <tableColumns count="14">
     <tableColumn id="1" name="序列"/>
     <tableColumn id="2" name="名字"/>
@@ -1465,10 +1476,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N23"/>
+  <dimension ref="A1:N24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1701,7 +1712,7 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
         <v>76</v>
@@ -1745,7 +1756,7 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
         <v>43</v>
@@ -2009,13 +2020,13 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A13">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>68</v>
+        <v>89</v>
       </c>
       <c r="C13" t="s">
-        <v>69</v>
+        <v>90</v>
       </c>
       <c r="D13">
         <v>0</v>
@@ -2027,36 +2038,39 @@
         <v>0</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="H13" s="5" t="s">
         <v>67</v>
       </c>
       <c r="I13">
-        <v>-60</v>
+        <v>0</v>
       </c>
       <c r="J13">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="K13">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="L13">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="M13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N13" t="s">
-        <v>70</v>
+        <v>91</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A14">
-        <v>32</v>
+        <v>31</v>
+      </c>
+      <c r="B14" t="s">
+        <v>68</v>
       </c>
       <c r="C14" t="s">
-        <v>11</v>
+        <v>69</v>
       </c>
       <c r="D14">
         <v>0</v>
@@ -2068,36 +2082,36 @@
         <v>0</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="I14">
-        <v>-184</v>
+        <v>-60</v>
       </c>
       <c r="J14">
-        <v>120</v>
+        <v>60</v>
       </c>
       <c r="K14">
-        <v>28</v>
+        <v>50</v>
       </c>
       <c r="L14">
-        <v>28</v>
+        <v>50</v>
       </c>
       <c r="M14">
         <v>0</v>
       </c>
       <c r="N14" t="s">
-        <v>12</v>
+        <v>70</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A15">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C15" t="s">
-        <v>81</v>
+        <v>11</v>
       </c>
       <c r="D15">
         <v>0</v>
@@ -2118,27 +2132,27 @@
         <v>-184</v>
       </c>
       <c r="J15">
-        <v>62</v>
+        <v>120</v>
       </c>
       <c r="K15">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="L15">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="M15">
         <v>0</v>
       </c>
       <c r="N15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A16">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C16" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D16">
         <v>0</v>
@@ -2159,30 +2173,27 @@
         <v>-184</v>
       </c>
       <c r="J16">
-        <v>155</v>
+        <v>62</v>
       </c>
       <c r="K16">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="L16">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="M16">
         <v>0</v>
       </c>
       <c r="N16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A17">
-        <v>36</v>
-      </c>
-      <c r="B17" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="C17" t="s">
-        <v>16</v>
+        <v>80</v>
       </c>
       <c r="D17">
         <v>0</v>
@@ -2191,7 +2202,7 @@
         <v>0</v>
       </c>
       <c r="F17">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="G17" s="5" t="s">
         <v>67</v>
@@ -2200,33 +2211,33 @@
         <v>66</v>
       </c>
       <c r="I17">
-        <v>0</v>
+        <v>-184</v>
       </c>
       <c r="J17">
-        <v>0</v>
+        <v>155</v>
       </c>
       <c r="K17">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="L17">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="M17">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N17" t="s">
-        <v>75</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A18">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B18" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C18" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D18">
         <v>0</v>
@@ -2234,8 +2245,8 @@
       <c r="E18">
         <v>0</v>
       </c>
-      <c r="F18" s="3">
-        <v>50</v>
+      <c r="F18">
+        <v>8</v>
       </c>
       <c r="G18" s="5" t="s">
         <v>67</v>
@@ -2259,18 +2270,18 @@
         <v>2</v>
       </c>
       <c r="N18" t="s">
-        <v>19</v>
+        <v>75</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A19">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B19" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C19" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D19">
         <v>0</v>
@@ -2303,18 +2314,18 @@
         <v>2</v>
       </c>
       <c r="N19" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A20">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B20" t="s">
-        <v>45</v>
+        <v>20</v>
       </c>
       <c r="C20" t="s">
-        <v>46</v>
+        <v>21</v>
       </c>
       <c r="D20">
         <v>0</v>
@@ -2322,8 +2333,8 @@
       <c r="E20">
         <v>0</v>
       </c>
-      <c r="F20">
-        <v>5</v>
+      <c r="F20" s="3">
+        <v>50</v>
       </c>
       <c r="G20" s="5" t="s">
         <v>67</v>
@@ -2347,27 +2358,27 @@
         <v>2</v>
       </c>
       <c r="N20" t="s">
-        <v>48</v>
+        <v>22</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A21">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B21" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
       <c r="C21" t="s">
-        <v>24</v>
+        <v>46</v>
       </c>
       <c r="D21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E21">
-        <v>1004</v>
+        <v>0</v>
       </c>
       <c r="F21">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="G21" s="5" t="s">
         <v>67</v>
@@ -2391,27 +2402,27 @@
         <v>2</v>
       </c>
       <c r="N21" t="s">
-        <v>25</v>
+        <v>48</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A22">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B22" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="C22" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="D22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E22">
-        <v>0</v>
-      </c>
-      <c r="F22" s="3">
-        <v>50</v>
+        <v>1004</v>
+      </c>
+      <c r="F22">
+        <v>20</v>
       </c>
       <c r="G22" s="5" t="s">
         <v>67</v>
@@ -2435,18 +2446,18 @@
         <v>2</v>
       </c>
       <c r="N22" t="s">
-        <v>44</v>
+        <v>25</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A23">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B23" t="s">
-        <v>73</v>
+        <v>40</v>
       </c>
       <c r="C23" t="s">
-        <v>74</v>
+        <v>41</v>
       </c>
       <c r="D23">
         <v>0</v>
@@ -2454,14 +2465,14 @@
       <c r="E23">
         <v>0</v>
       </c>
-      <c r="F23">
-        <v>0</v>
+      <c r="F23" s="3">
+        <v>50</v>
       </c>
       <c r="G23" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="H23" s="5" t="s">
         <v>66</v>
-      </c>
-      <c r="H23" s="5" t="s">
-        <v>67</v>
       </c>
       <c r="I23">
         <v>0</v>
@@ -2479,6 +2490,50 @@
         <v>2</v>
       </c>
       <c r="N23" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A24">
+        <v>43</v>
+      </c>
+      <c r="B24" t="s">
+        <v>73</v>
+      </c>
+      <c r="C24" t="s">
+        <v>74</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="H24" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="I24">
+        <v>0</v>
+      </c>
+      <c r="J24">
+        <v>0</v>
+      </c>
+      <c r="K24">
+        <v>0</v>
+      </c>
+      <c r="L24">
+        <v>0</v>
+      </c>
+      <c r="M24">
+        <v>2</v>
+      </c>
+      <c r="N24" t="s">
         <v>47</v>
       </c>
     </row>

</xml_diff>

<commit_message>
adjust button on role form
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/MainIcon.xlsx
+++ b/ConfigData/Xlsx/MainIcon.xlsx
@@ -81,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="89">
   <si>
     <t>打开主菜单(ESC)</t>
   </si>
@@ -336,19 +336,7 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>传记</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>进入传记</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>MainIcon3</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>MainIcon9</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
@@ -1133,8 +1121,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:N24" totalsRowShown="0" headerRowDxfId="2">
-  <autoFilter ref="A1:N24"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:N23" totalsRowShown="0" headerRowDxfId="2">
+  <autoFilter ref="A1:N23"/>
   <tableColumns count="14">
     <tableColumn id="1" name="序列"/>
     <tableColumn id="2" name="名字"/>
@@ -1476,10 +1464,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N24"/>
+  <dimension ref="A1:N23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1674,7 +1662,7 @@
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -1712,13 +1700,13 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>76</v>
+        <v>43</v>
       </c>
       <c r="C6" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -1751,18 +1739,18 @@
         <v>1</v>
       </c>
       <c r="N6" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A7">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>43</v>
+        <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -1771,13 +1759,13 @@
         <v>0</v>
       </c>
       <c r="F7">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G7" s="5" t="s">
         <v>67</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I7">
         <v>0</v>
@@ -1795,18 +1783,18 @@
         <v>1</v>
       </c>
       <c r="N7" t="s">
-        <v>78</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A8">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -1815,7 +1803,7 @@
         <v>0</v>
       </c>
       <c r="F8">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G8" s="5" t="s">
         <v>67</v>
@@ -1839,18 +1827,18 @@
         <v>1</v>
       </c>
       <c r="N8" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A9">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>6</v>
+        <v>72</v>
       </c>
       <c r="C9" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -1862,10 +1850,10 @@
         <v>2</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="I9">
         <v>0</v>
@@ -1883,18 +1871,18 @@
         <v>1</v>
       </c>
       <c r="N9" t="s">
-        <v>7</v>
+        <v>71</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A10">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>72</v>
+        <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -1903,10 +1891,10 @@
         <v>0</v>
       </c>
       <c r="F10">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="H10" s="5" t="s">
         <v>67</v>
@@ -1927,18 +1915,18 @@
         <v>1</v>
       </c>
       <c r="N10" t="s">
-        <v>71</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A11">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>8</v>
+        <v>42</v>
       </c>
       <c r="C11" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D11">
         <v>0</v>
@@ -1947,7 +1935,7 @@
         <v>0</v>
       </c>
       <c r="F11">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G11" s="5" t="s">
         <v>67</v>
@@ -1971,18 +1959,18 @@
         <v>1</v>
       </c>
       <c r="N11" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A12">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>42</v>
+        <v>86</v>
       </c>
       <c r="C12" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="D12">
         <v>0</v>
@@ -1991,7 +1979,7 @@
         <v>0</v>
       </c>
       <c r="F12">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G12" s="5" t="s">
         <v>67</v>
@@ -2015,18 +2003,18 @@
         <v>1</v>
       </c>
       <c r="N12" t="s">
-        <v>10</v>
+        <v>88</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A13">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="B13" t="s">
-        <v>89</v>
+        <v>68</v>
       </c>
       <c r="C13" t="s">
-        <v>90</v>
+        <v>69</v>
       </c>
       <c r="D13">
         <v>0</v>
@@ -2038,39 +2026,36 @@
         <v>0</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H13" s="5" t="s">
         <v>67</v>
       </c>
       <c r="I13">
-        <v>0</v>
+        <v>-60</v>
       </c>
       <c r="J13">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="K13">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="L13">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="M13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N13" t="s">
-        <v>91</v>
+        <v>70</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A14">
-        <v>31</v>
-      </c>
-      <c r="B14" t="s">
-        <v>68</v>
+        <v>32</v>
       </c>
       <c r="C14" t="s">
-        <v>69</v>
+        <v>11</v>
       </c>
       <c r="D14">
         <v>0</v>
@@ -2082,36 +2067,36 @@
         <v>0</v>
       </c>
       <c r="G14" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="H14" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="H14" s="5" t="s">
-        <v>67</v>
-      </c>
       <c r="I14">
-        <v>-60</v>
+        <v>-184</v>
       </c>
       <c r="J14">
-        <v>60</v>
+        <v>120</v>
       </c>
       <c r="K14">
-        <v>50</v>
+        <v>28</v>
       </c>
       <c r="L14">
-        <v>50</v>
+        <v>28</v>
       </c>
       <c r="M14">
         <v>0</v>
       </c>
       <c r="N14" t="s">
-        <v>70</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A15">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C15" t="s">
-        <v>11</v>
+        <v>78</v>
       </c>
       <c r="D15">
         <v>0</v>
@@ -2132,27 +2117,27 @@
         <v>-184</v>
       </c>
       <c r="J15">
-        <v>120</v>
+        <v>62</v>
       </c>
       <c r="K15">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="L15">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="M15">
         <v>0</v>
       </c>
       <c r="N15" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A16">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C16" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D16">
         <v>0</v>
@@ -2173,27 +2158,30 @@
         <v>-184</v>
       </c>
       <c r="J16">
-        <v>62</v>
+        <v>155</v>
       </c>
       <c r="K16">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="L16">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="M16">
         <v>0</v>
       </c>
       <c r="N16" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A17">
-        <v>34</v>
+        <v>36</v>
+      </c>
+      <c r="B17" t="s">
+        <v>15</v>
       </c>
       <c r="C17" t="s">
-        <v>80</v>
+        <v>16</v>
       </c>
       <c r="D17">
         <v>0</v>
@@ -2202,7 +2190,7 @@
         <v>0</v>
       </c>
       <c r="F17">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G17" s="5" t="s">
         <v>67</v>
@@ -2211,33 +2199,33 @@
         <v>66</v>
       </c>
       <c r="I17">
-        <v>-184</v>
+        <v>0</v>
       </c>
       <c r="J17">
-        <v>155</v>
+        <v>0</v>
       </c>
       <c r="K17">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="L17">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="M17">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N17" t="s">
-        <v>14</v>
+        <v>75</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A18">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B18" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C18" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D18">
         <v>0</v>
@@ -2245,8 +2233,8 @@
       <c r="E18">
         <v>0</v>
       </c>
-      <c r="F18">
-        <v>8</v>
+      <c r="F18" s="3">
+        <v>50</v>
       </c>
       <c r="G18" s="5" t="s">
         <v>67</v>
@@ -2270,18 +2258,18 @@
         <v>2</v>
       </c>
       <c r="N18" t="s">
-        <v>75</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A19">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B19" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C19" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D19">
         <v>0</v>
@@ -2314,18 +2302,18 @@
         <v>2</v>
       </c>
       <c r="N19" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A20">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B20" t="s">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="C20" t="s">
-        <v>21</v>
+        <v>46</v>
       </c>
       <c r="D20">
         <v>0</v>
@@ -2333,8 +2321,8 @@
       <c r="E20">
         <v>0</v>
       </c>
-      <c r="F20" s="3">
-        <v>50</v>
+      <c r="F20">
+        <v>5</v>
       </c>
       <c r="G20" s="5" t="s">
         <v>67</v>
@@ -2358,27 +2346,27 @@
         <v>2</v>
       </c>
       <c r="N20" t="s">
-        <v>22</v>
+        <v>48</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A21">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B21" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="C21" t="s">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="D21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E21">
-        <v>0</v>
+        <v>1004</v>
       </c>
       <c r="F21">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="G21" s="5" t="s">
         <v>67</v>
@@ -2402,27 +2390,27 @@
         <v>2</v>
       </c>
       <c r="N21" t="s">
-        <v>48</v>
+        <v>25</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A22">
+        <v>42</v>
+      </c>
+      <c r="B22" t="s">
+        <v>40</v>
+      </c>
+      <c r="C22" t="s">
         <v>41</v>
       </c>
-      <c r="B22" t="s">
-        <v>23</v>
-      </c>
-      <c r="C22" t="s">
-        <v>24</v>
-      </c>
       <c r="D22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E22">
-        <v>1004</v>
-      </c>
-      <c r="F22">
-        <v>20</v>
+        <v>0</v>
+      </c>
+      <c r="F22" s="3">
+        <v>50</v>
       </c>
       <c r="G22" s="5" t="s">
         <v>67</v>
@@ -2446,18 +2434,18 @@
         <v>2</v>
       </c>
       <c r="N22" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A23">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B23" t="s">
-        <v>40</v>
+        <v>73</v>
       </c>
       <c r="C23" t="s">
-        <v>41</v>
+        <v>74</v>
       </c>
       <c r="D23">
         <v>0</v>
@@ -2465,14 +2453,14 @@
       <c r="E23">
         <v>0</v>
       </c>
-      <c r="F23" s="3">
-        <v>50</v>
+      <c r="F23">
+        <v>0</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H23" s="5" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="I23">
         <v>0</v>
@@ -2490,50 +2478,6 @@
         <v>2</v>
       </c>
       <c r="N23" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A24">
-        <v>43</v>
-      </c>
-      <c r="B24" t="s">
-        <v>73</v>
-      </c>
-      <c r="C24" t="s">
-        <v>74</v>
-      </c>
-      <c r="D24">
-        <v>0</v>
-      </c>
-      <c r="E24">
-        <v>0</v>
-      </c>
-      <c r="F24">
-        <v>0</v>
-      </c>
-      <c r="G24" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="H24" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="I24">
-        <v>0</v>
-      </c>
-      <c r="J24">
-        <v>0</v>
-      </c>
-      <c r="K24">
-        <v>0</v>
-      </c>
-      <c r="L24">
-        <v>0</v>
-      </c>
-      <c r="M24">
-        <v>2</v>
-      </c>
-      <c r="N24" t="s">
         <v>47</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add the blackstone form
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/MainIcon.xlsx
+++ b/ConfigData/Xlsx/MainIcon.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19330"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TOMClassic\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{3FE312D4-D570-4561-9200-70321536B183}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{68E6AE87-6AE5-4546-A1A5-DB1EA0BC76CC}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -82,7 +82,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="92">
   <si>
     <t>打开主菜单(ESC)</t>
   </si>
@@ -386,6 +386,18 @@
   </si>
   <si>
     <t>MainIcon10</t>
+  </si>
+  <si>
+    <t>SideButton8</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>黑曜石</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>打开黑曜石面板</t>
+    <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1125,8 +1137,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="表1" displayName="表1" ref="A1:N23" totalsRowShown="0" headerRowDxfId="2">
-  <autoFilter ref="A1:N23" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="表1" displayName="表1" ref="A1:N24" totalsRowShown="0" headerRowDxfId="2">
+  <autoFilter ref="A1:N24" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="14">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="序列"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="名字"/>
@@ -1468,10 +1480,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N23"/>
+  <dimension ref="A1:N24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2485,6 +2497,50 @@
         <v>47</v>
       </c>
     </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A24">
+        <v>44</v>
+      </c>
+      <c r="B24" t="s">
+        <v>90</v>
+      </c>
+      <c r="C24" t="s">
+        <v>91</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="H24" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="I24">
+        <v>0</v>
+      </c>
+      <c r="J24">
+        <v>0</v>
+      </c>
+      <c r="K24">
+        <v>0</v>
+      </c>
+      <c r="L24">
+        <v>0</v>
+      </c>
+      <c r="M24">
+        <v>2</v>
+      </c>
+      <c r="N24" t="s">
+        <v>89</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>